<commit_message>
Can create a train, including scheduling a time to dispatch, and calculation an authority and estimated arrival time
</commit_message>
<xml_diff>
--- a/CTC_Office/Green_Line_Layout.xlsx
+++ b/CTC_Office/Green_Line_Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaseckrich/Documents/Classes/ECE 1140/ECE1140_TermProject/CTC_Office/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C5C711-1194-4D43-9568-6549055E9EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706493A-6D44-B44D-92C3-DB3700973583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3560" windowWidth="38400" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -741,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L158"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -849,7 +849,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I35" si="0">E3*D3/100</f>
+        <f t="shared" ref="I3:I34" si="0">E3*D3/100</f>
         <v>0.5</v>
       </c>
       <c r="J3" s="4">
@@ -857,7 +857,7 @@
         <v>0.5</v>
       </c>
       <c r="K3" s="6">
-        <f t="shared" ref="K3:K35" si="1">D3*(1/(F3*1000/(60*60)))</f>
+        <f t="shared" ref="K3:K34" si="1">D3*(1/(F3*1000/(60*60)))</f>
         <v>8</v>
       </c>
       <c r="L3" s="7">
@@ -866,7 +866,7 @@
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="str">
-        <f t="shared" ref="A4:A39" si="2">A3</f>
+        <f t="shared" ref="A4:A38" si="2">A3</f>
         <v>Green</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -895,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J36" si="3">I4+J3</f>
+        <f t="shared" ref="J4:J35" si="3">I4+J3</f>
         <v>1.5</v>
       </c>
       <c r="K4" s="6">
@@ -1058,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f>A8</f>
         <v>Green</v>
@@ -1066,8 +1066,8 @@
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4">
-        <v>151</v>
+      <c r="C9" s="5">
+        <v>7</v>
       </c>
       <c r="D9" s="4">
         <v>50</v>
@@ -1078,63 +1078,63 @@
       <c r="F9" s="4">
         <v>45</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4">
-        <f t="shared" si="0"/>
+        <f>E9*D9/100</f>
         <v>2.5</v>
       </c>
       <c r="J9" s="4">
-        <f>I9+J8</f>
-        <v>14.5</v>
+        <f>I9+J153</f>
+        <v>17</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L9" s="7">
-        <v>6</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="str">
-        <f>A8</f>
+        <f t="shared" si="2"/>
         <v>Green</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5">
-        <v>7</v>
+      <c r="C10" s="4">
+        <v>8</v>
       </c>
       <c r="D10" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E10" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4">
         <v>45</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4">
-        <f>E10*D10/100</f>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J10" s="4">
-        <f>I10+J9</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L10" s="7">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1143,36 +1143,40 @@
         <v>17</v>
       </c>
       <c r="C11" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4">
         <v>100</v>
       </c>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="F11" s="4">
         <v>45</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L11" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1180,38 +1184,34 @@
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4">
-        <v>9</v>
+      <c r="C12" s="5">
+        <v>10</v>
       </c>
       <c r="D12" s="4">
         <v>100</v>
       </c>
       <c r="E12" s="4">
-        <v>-5</v>
+        <v>-4.5</v>
       </c>
       <c r="F12" s="4">
         <v>45</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="4">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-4.5</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>7.5</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L12" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1222,14 +1222,14 @@
       <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5">
-        <v>10</v>
+      <c r="C13" s="4">
+        <v>11</v>
       </c>
       <c r="D13" s="4">
         <v>100</v>
       </c>
       <c r="E13" s="4">
-        <v>-4.5</v>
+        <v>-4</v>
       </c>
       <c r="F13" s="4">
         <v>45</v>
@@ -1238,18 +1238,18 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4">
         <f t="shared" si="0"/>
-        <v>-4.5</v>
+        <v>-4</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="K13" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L13" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1260,34 +1260,33 @@
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4">
-        <v>11</v>
+      <c r="C14" s="5">
+        <v>12</v>
       </c>
       <c r="D14" s="4">
         <v>100</v>
       </c>
       <c r="E14" s="4">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="F14" s="4">
         <v>45</v>
       </c>
-      <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L14" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1296,24 +1295,27 @@
         <v>Green</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>13</v>
       </c>
       <c r="D15" s="4">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E15" s="4">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>45</v>
+        <v>70</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="3"/>
@@ -1321,10 +1323,10 @@
       </c>
       <c r="K15" s="6">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="L15" s="7">
-        <v>11</v>
+        <v>7.7142857142857153</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1336,7 +1338,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" s="4">
         <v>150</v>
@@ -1347,9 +1349,7 @@
       <c r="F16" s="4">
         <v>70</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4">
         <f t="shared" si="0"/>
@@ -1364,7 +1364,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1375,8 +1375,8 @@
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4">
-        <v>14</v>
+      <c r="C17" s="5">
+        <v>15</v>
       </c>
       <c r="D17" s="4">
         <v>150</v>
@@ -1402,10 +1402,10 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1413,8 +1413,8 @@
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="5">
-        <v>15</v>
+      <c r="C18" s="4">
+        <v>16</v>
       </c>
       <c r="D18" s="4">
         <v>150</v>
@@ -1425,8 +1425,12 @@
       <c r="F18" s="4">
         <v>70</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="G18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="I18" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1440,19 +1444,19 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="4">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="C19" s="5">
+        <v>17</v>
       </c>
       <c r="D19" s="4">
         <v>150</v>
@@ -1461,14 +1465,10 @@
         <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>70</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
       <c r="I19" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1479,10 +1479,10 @@
       </c>
       <c r="K19" s="6">
         <f t="shared" si="1"/>
-        <v>7.7142857142857153</v>
+        <v>9</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1493,8 +1493,8 @@
       <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="5">
-        <v>17</v>
+      <c r="C20" s="4">
+        <v>18</v>
       </c>
       <c r="D20" s="4">
         <v>150</v>
@@ -1520,10 +1520,10 @@
         <v>9</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1532,7 +1532,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21" s="4">
         <v>150</v>
@@ -1543,7 +1543,9 @@
       <c r="F21" s="4">
         <v>60</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4">
         <f t="shared" si="0"/>
@@ -1558,10 +1560,10 @@
         <v>9</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1569,8 +1571,8 @@
       <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="4">
-        <v>19</v>
+      <c r="C22" s="5">
+        <v>20</v>
       </c>
       <c r="D22" s="4">
         <v>150</v>
@@ -1581,9 +1583,7 @@
       <c r="F22" s="4">
         <v>60</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4">
         <f t="shared" si="0"/>
@@ -1598,7 +1598,7 @@
         <v>9</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1607,19 +1607,19 @@
         <v>Green</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="5">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="C23" s="4">
+        <v>21</v>
       </c>
       <c r="D23" s="4">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
       </c>
       <c r="F23" s="4">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1633,13 +1633,13 @@
       </c>
       <c r="K23" s="6">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>15.428571428571431</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1647,8 +1647,8 @@
       <c r="B24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="4">
-        <v>21</v>
+      <c r="C24" s="5">
+        <v>22</v>
       </c>
       <c r="D24" s="4">
         <v>300</v>
@@ -1659,8 +1659,12 @@
       <c r="F24" s="4">
         <v>70</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="G24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="I24" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1674,10 +1678,10 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1685,8 +1689,8 @@
       <c r="B25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="5">
-        <v>22</v>
+      <c r="C25" s="4">
+        <v>23</v>
       </c>
       <c r="D25" s="4">
         <v>300</v>
@@ -1697,12 +1701,8 @@
       <c r="F25" s="4">
         <v>70</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1728,7 +1728,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" s="4">
         <v>300</v>
@@ -1754,7 +1754,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1765,11 +1765,11 @@
       <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="4">
-        <v>24</v>
+      <c r="C27" s="5">
+        <v>25</v>
       </c>
       <c r="D27" s="4">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -1789,10 +1789,10 @@
       </c>
       <c r="K27" s="6">
         <f t="shared" si="1"/>
-        <v>15.428571428571431</v>
+        <v>10.285714285714286</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1803,11 +1803,11 @@
       <c r="B28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="5">
-        <v>25</v>
+      <c r="C28" s="4">
+        <v>26</v>
       </c>
       <c r="D28" s="4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E28" s="4">
         <v>0</v>
@@ -1827,10 +1827,10 @@
       </c>
       <c r="K28" s="6">
         <f t="shared" si="1"/>
-        <v>10.285714285714286</v>
+        <v>5.1428571428571432</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1841,17 +1841,17 @@
       <c r="B29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="4">
-        <v>26</v>
+      <c r="C29" s="5">
+        <v>27</v>
       </c>
       <c r="D29" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1865,10 +1865,10 @@
       </c>
       <c r="K29" s="6">
         <f t="shared" si="1"/>
-        <v>5.1428571428571432</v>
+        <v>6</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1879,8 +1879,8 @@
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="5">
-        <v>27</v>
+      <c r="C30" s="4">
+        <v>28</v>
       </c>
       <c r="D30" s="4">
         <v>50</v>
@@ -1891,7 +1891,9 @@
       <c r="F30" s="4">
         <v>30</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4">
         <f t="shared" si="0"/>
@@ -1906,7 +1908,7 @@
         <v>6</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1915,10 +1917,10 @@
         <v>Green</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C31" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D31" s="4">
         <v>50</v>
@@ -1929,9 +1931,7 @@
       <c r="F31" s="4">
         <v>30</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4">
         <f t="shared" si="0"/>
@@ -1945,8 +1945,8 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L31" s="7" t="s">
-        <v>43</v>
+      <c r="L31" s="7">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1957,8 +1957,8 @@
       <c r="B32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="4">
-        <v>29</v>
+      <c r="C32" s="5">
+        <v>30</v>
       </c>
       <c r="D32" s="4">
         <v>50</v>
@@ -1984,10 +1984,10 @@
         <v>6</v>
       </c>
       <c r="L32" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -1995,8 +1995,8 @@
       <c r="B33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="5">
-        <v>30</v>
+      <c r="C33" s="4">
+        <v>31</v>
       </c>
       <c r="D33" s="4">
         <v>50</v>
@@ -2007,8 +2007,12 @@
       <c r="F33" s="4">
         <v>30</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="G33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I33" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2022,10 +2026,10 @@
         <v>6</v>
       </c>
       <c r="L33" s="7">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2033,8 +2037,8 @@
       <c r="B34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="4">
-        <v>31</v>
+      <c r="C34" s="5">
+        <v>32</v>
       </c>
       <c r="D34" s="4">
         <v>50</v>
@@ -2045,12 +2049,8 @@
       <c r="F34" s="4">
         <v>30</v>
       </c>
-      <c r="G34" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
       <c r="I34" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>6</v>
       </c>
       <c r="L34" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2073,10 +2073,10 @@
         <v>Green</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="5">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="C35" s="4">
+        <v>33</v>
       </c>
       <c r="D35" s="4">
         <v>50</v>
@@ -2090,7 +2090,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I35:I66" si="4">E35*D35/100</f>
         <v>0</v>
       </c>
       <c r="J35" s="4">
@@ -2098,11 +2098,11 @@
         <v>0.5</v>
       </c>
       <c r="K35" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K35:K66" si="5">D35*(1/(F35*1000/(60*60)))</f>
         <v>6</v>
       </c>
       <c r="L35" s="7">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2114,7 +2114,7 @@
         <v>46</v>
       </c>
       <c r="C36" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D36" s="4">
         <v>50</v>
@@ -2128,19 +2128,19 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4">
-        <f t="shared" ref="I36:I67" si="4">E36*D36/100</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J36" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J36:J67" si="6">I36+J35</f>
         <v>0.5</v>
       </c>
       <c r="K36" s="6">
-        <f t="shared" ref="K36:K67" si="5">D36*(1/(F36*1000/(60*60)))</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L36" s="7">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2151,8 +2151,8 @@
       <c r="B37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="4">
-        <v>34</v>
+      <c r="C37" s="5">
+        <v>35</v>
       </c>
       <c r="D37" s="4">
         <v>50</v>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" ref="J37:J68" si="6">I37+J36</f>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="K37" s="6">
@@ -2178,7 +2178,7 @@
         <v>6</v>
       </c>
       <c r="L37" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2187,10 +2187,10 @@
         <v>Green</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="5">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="C38" s="4">
+        <v>36</v>
       </c>
       <c r="D38" s="4">
         <v>50</v>
@@ -2201,7 +2201,9 @@
       <c r="F38" s="4">
         <v>30</v>
       </c>
-      <c r="G38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4">
         <f t="shared" si="4"/>
@@ -2216,19 +2218,19 @@
         <v>6</v>
       </c>
       <c r="L38" s="7">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f>A35</f>
         <v>Green</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C39" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D39" s="4">
         <v>50</v>
@@ -2256,19 +2258,19 @@
         <v>6</v>
       </c>
       <c r="L39" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="str">
-        <f>A36</f>
+        <f t="shared" ref="A40:A71" si="7">A39</f>
         <v>Green</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="4">
-        <v>37</v>
+      <c r="C40" s="5">
+        <v>38</v>
       </c>
       <c r="D40" s="4">
         <v>50</v>
@@ -2296,19 +2298,19 @@
         <v>6</v>
       </c>
       <c r="L40" s="7">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="str">
-        <f t="shared" ref="A41:A72" si="7">A40</f>
+        <f t="shared" si="7"/>
         <v>Green</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="5">
-        <v>38</v>
+      <c r="C41" s="4">
+        <v>39</v>
       </c>
       <c r="D41" s="4">
         <v>50</v>
@@ -2319,10 +2321,12 @@
       <c r="F41" s="4">
         <v>30</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H41" s="4"/>
+      <c r="G41" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I41" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2336,10 +2340,10 @@
         <v>6</v>
       </c>
       <c r="L41" s="7">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2348,7 +2352,7 @@
         <v>47</v>
       </c>
       <c r="C42" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D42" s="4">
         <v>50</v>
@@ -2359,12 +2363,10 @@
       <c r="F42" s="4">
         <v>30</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="4"/>
       <c r="I42" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2378,7 +2380,7 @@
         <v>6</v>
       </c>
       <c r="L42" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2389,8 +2391,8 @@
       <c r="B43" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="4">
-        <v>40</v>
+      <c r="C43" s="5">
+        <v>41</v>
       </c>
       <c r="D43" s="4">
         <v>50</v>
@@ -2418,7 +2420,7 @@
         <v>6</v>
       </c>
       <c r="L43" s="7">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2429,8 +2431,8 @@
       <c r="B44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="5">
-        <v>41</v>
+      <c r="C44" s="4">
+        <v>42</v>
       </c>
       <c r="D44" s="4">
         <v>50</v>
@@ -2458,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="L44" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2470,7 +2472,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D45" s="4">
         <v>50</v>
@@ -2498,7 +2500,7 @@
         <v>6</v>
       </c>
       <c r="L45" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2509,8 +2511,8 @@
       <c r="B46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="4">
-        <v>43</v>
+      <c r="C46" s="5">
+        <v>44</v>
       </c>
       <c r="D46" s="4">
         <v>50</v>
@@ -2538,7 +2540,7 @@
         <v>6</v>
       </c>
       <c r="L46" s="7">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2549,8 +2551,8 @@
       <c r="B47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="5">
-        <v>44</v>
+      <c r="C47" s="4">
+        <v>45</v>
       </c>
       <c r="D47" s="4">
         <v>50</v>
@@ -2578,7 +2580,7 @@
         <v>6</v>
       </c>
       <c r="L47" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2590,7 +2592,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D48" s="4">
         <v>50</v>
@@ -2618,7 +2620,7 @@
         <v>6</v>
       </c>
       <c r="L48" s="7">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2629,8 +2631,8 @@
       <c r="B49" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="4">
-        <v>46</v>
+      <c r="C49" s="5">
+        <v>47</v>
       </c>
       <c r="D49" s="4">
         <v>50</v>
@@ -2658,10 +2660,10 @@
         <v>6</v>
       </c>
       <c r="L49" s="7">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2669,8 +2671,8 @@
       <c r="B50" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="5">
-        <v>47</v>
+      <c r="C50" s="4">
+        <v>48</v>
       </c>
       <c r="D50" s="4">
         <v>50</v>
@@ -2681,10 +2683,12 @@
       <c r="F50" s="4">
         <v>30</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H50" s="4"/>
+      <c r="G50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I50" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2698,10 +2702,10 @@
         <v>6</v>
       </c>
       <c r="L50" s="7">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -2710,7 +2714,7 @@
         <v>47</v>
       </c>
       <c r="C51" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D51" s="4">
         <v>50</v>
@@ -2721,12 +2725,10 @@
       <c r="F51" s="4">
         <v>30</v>
       </c>
-      <c r="G51" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G51" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H51" s="4"/>
       <c r="I51" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2740,7 +2742,7 @@
         <v>6</v>
       </c>
       <c r="L51" s="7">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2751,8 +2753,8 @@
       <c r="B52" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="4">
-        <v>49</v>
+      <c r="C52" s="5">
+        <v>50</v>
       </c>
       <c r="D52" s="4">
         <v>50</v>
@@ -2780,7 +2782,7 @@
         <v>6</v>
       </c>
       <c r="L52" s="7">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2791,8 +2793,8 @@
       <c r="B53" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="5">
-        <v>50</v>
+      <c r="C53" s="4">
+        <v>51</v>
       </c>
       <c r="D53" s="4">
         <v>50</v>
@@ -2820,7 +2822,7 @@
         <v>6</v>
       </c>
       <c r="L53" s="7">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2832,7 +2834,7 @@
         <v>47</v>
       </c>
       <c r="C54" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D54" s="4">
         <v>50</v>
@@ -2860,7 +2862,7 @@
         <v>6</v>
       </c>
       <c r="L54" s="7">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2871,8 +2873,8 @@
       <c r="B55" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="4">
-        <v>52</v>
+      <c r="C55" s="5">
+        <v>53</v>
       </c>
       <c r="D55" s="4">
         <v>50</v>
@@ -2900,7 +2902,7 @@
         <v>6</v>
       </c>
       <c r="L55" s="7">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2911,8 +2913,8 @@
       <c r="B56" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="5">
-        <v>53</v>
+      <c r="C56" s="4">
+        <v>54</v>
       </c>
       <c r="D56" s="4">
         <v>50</v>
@@ -2940,7 +2942,7 @@
         <v>6</v>
       </c>
       <c r="L56" s="7">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2952,7 +2954,7 @@
         <v>47</v>
       </c>
       <c r="C57" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D57" s="4">
         <v>50</v>
@@ -2980,7 +2982,7 @@
         <v>6</v>
       </c>
       <c r="L57" s="7">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2991,8 +2993,8 @@
       <c r="B58" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C58" s="4">
-        <v>55</v>
+      <c r="C58" s="5">
+        <v>56</v>
       </c>
       <c r="D58" s="4">
         <v>50</v>
@@ -3020,10 +3022,10 @@
         <v>6</v>
       </c>
       <c r="L58" s="7">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3031,8 +3033,8 @@
       <c r="B59" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="5">
-        <v>56</v>
+      <c r="C59" s="4">
+        <v>57</v>
       </c>
       <c r="D59" s="4">
         <v>50</v>
@@ -3043,10 +3045,12 @@
       <c r="F59" s="4">
         <v>30</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H59" s="4"/>
+      <c r="G59" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I59" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3059,20 +3063,20 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="L59" s="7">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="L59" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C60" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D60" s="4">
         <v>50</v>
@@ -3083,12 +3087,8 @@
       <c r="F60" s="4">
         <v>30</v>
       </c>
-      <c r="G60" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G60" s="8"/>
+      <c r="H60" s="4"/>
       <c r="I60" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3101,8 +3101,8 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="L60" s="7" t="s">
-        <v>52</v>
+      <c r="L60" s="7">
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3113,8 +3113,8 @@
       <c r="B61" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="4">
-        <v>58</v>
+      <c r="C61" s="5">
+        <v>59</v>
       </c>
       <c r="D61" s="4">
         <v>50</v>
@@ -3125,7 +3125,7 @@
       <c r="F61" s="4">
         <v>30</v>
       </c>
-      <c r="G61" s="8"/>
+      <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4">
         <f t="shared" si="4"/>
@@ -3140,7 +3140,7 @@
         <v>6</v>
       </c>
       <c r="L61" s="7">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3151,8 +3151,8 @@
       <c r="B62" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="5">
-        <v>59</v>
+      <c r="C62" s="4">
+        <v>60</v>
       </c>
       <c r="D62" s="4">
         <v>50</v>
@@ -3178,7 +3178,7 @@
         <v>6</v>
       </c>
       <c r="L62" s="7">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3190,7 +3190,7 @@
         <v>53</v>
       </c>
       <c r="C63" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D63" s="4">
         <v>50</v>
@@ -3216,7 +3216,7 @@
         <v>6</v>
       </c>
       <c r="L63" s="7">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3227,8 +3227,8 @@
       <c r="B64" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C64" s="4">
-        <v>61</v>
+      <c r="C64" s="5">
+        <v>62</v>
       </c>
       <c r="D64" s="4">
         <v>50</v>
@@ -3239,7 +3239,6 @@
       <c r="F64" s="4">
         <v>30</v>
       </c>
-      <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4">
         <f t="shared" si="4"/>
@@ -3254,28 +3253,31 @@
         <v>6</v>
       </c>
       <c r="L64" s="7">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C65" s="5">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="C65" s="4">
+        <v>63</v>
       </c>
       <c r="D65" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E65" s="4">
         <v>0</v>
       </c>
       <c r="F65" s="4">
-        <v>30</v>
+        <v>70</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4">
@@ -3288,13 +3290,13 @@
       </c>
       <c r="K65" s="6">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5.1428571428571432</v>
       </c>
       <c r="L65" s="7">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3303,7 +3305,7 @@
         <v>55</v>
       </c>
       <c r="C66" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D66" s="4">
         <v>100</v>
@@ -3314,9 +3316,7 @@
       <c r="F66" s="4">
         <v>70</v>
       </c>
-      <c r="G66" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4">
         <f t="shared" si="4"/>
@@ -3331,10 +3331,10 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="L66" s="7">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3342,11 +3342,11 @@
       <c r="B67" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C67" s="4">
-        <v>64</v>
+      <c r="C67" s="5">
+        <v>65</v>
       </c>
       <c r="D67" s="4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E67" s="4">
         <v>0</v>
@@ -3354,10 +3354,14 @@
       <c r="F67" s="4">
         <v>70</v>
       </c>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
+      <c r="G67" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I67" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I67:I98" si="8">E67*D67/100</f>
         <v>0</v>
       </c>
       <c r="J67" s="4">
@@ -3365,14 +3369,14 @@
         <v>0.5</v>
       </c>
       <c r="K67" s="6">
-        <f t="shared" si="5"/>
-        <v>5.1428571428571432</v>
+        <f t="shared" ref="K67:K98" si="9">D67*(1/(F67*1000/(60*60)))</f>
+        <v>10.285714285714286</v>
       </c>
       <c r="L67" s="7">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="str">
         <f t="shared" si="7"/>
         <v>Green</v>
@@ -3380,8 +3384,8 @@
       <c r="B68" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C68" s="5">
-        <v>65</v>
+      <c r="C68" s="4">
+        <v>66</v>
       </c>
       <c r="D68" s="4">
         <v>200</v>
@@ -3392,26 +3396,22 @@
       <c r="F68" s="4">
         <v>70</v>
       </c>
-      <c r="G68" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
       <c r="I68" s="4">
-        <f t="shared" ref="I68:I99" si="8">E68*D68/100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J68" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="J68:J99" si="10">I68+J67</f>
         <v>0.5</v>
       </c>
       <c r="K68" s="6">
-        <f t="shared" ref="K68:K99" si="9">D68*(1/(F68*1000/(60*60)))</f>
+        <f t="shared" si="9"/>
         <v>10.285714285714286</v>
       </c>
       <c r="L68" s="7">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3423,16 +3423,16 @@
         <v>55</v>
       </c>
       <c r="C69" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D69" s="4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E69" s="4">
         <v>0</v>
       </c>
       <c r="F69" s="4">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -3441,15 +3441,15 @@
         <v>0</v>
       </c>
       <c r="J69" s="4">
-        <f t="shared" ref="J69:J100" si="10">I69+J68</f>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="K69" s="6">
         <f t="shared" si="9"/>
-        <v>10.285714285714286</v>
+        <v>9</v>
       </c>
       <c r="L69" s="7">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3460,8 +3460,8 @@
       <c r="B70" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="4">
-        <v>67</v>
+      <c r="C70" s="5">
+        <v>68</v>
       </c>
       <c r="D70" s="4">
         <v>100</v>
@@ -3487,7 +3487,7 @@
         <v>9</v>
       </c>
       <c r="L70" s="7">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3496,10 +3496,10 @@
         <v>Green</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" s="5">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="C71" s="4">
+        <v>69</v>
       </c>
       <c r="D71" s="4">
         <v>100</v>
@@ -3525,19 +3525,19 @@
         <v>9</v>
       </c>
       <c r="L71" s="7">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A72:A103" si="11">A71</f>
         <v>Green</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C72" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D72" s="4">
         <v>100</v>
@@ -3563,19 +3563,19 @@
         <v>9</v>
       </c>
       <c r="L72" s="7">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="str">
-        <f t="shared" ref="A73:A104" si="11">A72</f>
+        <f t="shared" si="11"/>
         <v>Green</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C73" s="4">
-        <v>70</v>
+      <c r="C73" s="5">
+        <v>71</v>
       </c>
       <c r="D73" s="4">
         <v>100</v>
@@ -3601,7 +3601,7 @@
         <v>9</v>
       </c>
       <c r="L73" s="7">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3612,8 +3612,8 @@
       <c r="B74" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C74" s="5">
-        <v>71</v>
+      <c r="C74" s="4">
+        <v>72</v>
       </c>
       <c r="D74" s="4">
         <v>100</v>
@@ -3639,10 +3639,10 @@
         <v>9</v>
       </c>
       <c r="L74" s="7">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
@@ -3651,7 +3651,7 @@
         <v>57</v>
       </c>
       <c r="C75" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D75" s="4">
         <v>100</v>
@@ -3662,8 +3662,12 @@
       <c r="F75" s="4">
         <v>40</v>
       </c>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
+      <c r="G75" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I75" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3677,19 +3681,19 @@
         <v>9</v>
       </c>
       <c r="L75" s="7">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" s="4">
-        <v>73</v>
+        <v>59</v>
+      </c>
+      <c r="C76" s="5">
+        <v>74</v>
       </c>
       <c r="D76" s="4">
         <v>100</v>
@@ -3700,12 +3704,8 @@
       <c r="F76" s="4">
         <v>40</v>
       </c>
-      <c r="G76" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
       <c r="I76" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3719,7 +3719,7 @@
         <v>9</v>
       </c>
       <c r="L76" s="7">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3730,8 +3730,8 @@
       <c r="B77" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C77" s="5">
-        <v>74</v>
+      <c r="C77" s="4">
+        <v>75</v>
       </c>
       <c r="D77" s="4">
         <v>100</v>
@@ -3757,7 +3757,7 @@
         <v>9</v>
       </c>
       <c r="L77" s="7">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3769,7 +3769,7 @@
         <v>59</v>
       </c>
       <c r="C78" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D78" s="4">
         <v>100</v>
@@ -3795,31 +3795,35 @@
         <v>9</v>
       </c>
       <c r="L78" s="7">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C79" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D79" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E79" s="4">
         <v>0</v>
       </c>
       <c r="F79" s="4">
-        <v>40</v>
-      </c>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="I79" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3830,13 +3834,13 @@
       </c>
       <c r="K79" s="6">
         <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="L79" s="7">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>15.428571428571431</v>
+      </c>
+      <c r="L79" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
@@ -3844,8 +3848,8 @@
       <c r="B80" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C80" s="4">
-        <v>77</v>
+      <c r="C80" s="5">
+        <v>78</v>
       </c>
       <c r="D80" s="4">
         <v>300</v>
@@ -3856,12 +3860,8 @@
       <c r="F80" s="4">
         <v>70</v>
       </c>
-      <c r="G80" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
       <c r="I80" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3875,7 +3875,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L80" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3886,8 +3886,8 @@
       <c r="B81" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C81" s="5">
-        <v>78</v>
+      <c r="C81" s="4">
+        <v>79</v>
       </c>
       <c r="D81" s="4">
         <v>300</v>
@@ -3913,7 +3913,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L81" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3925,7 +3925,7 @@
         <v>60</v>
       </c>
       <c r="C82" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D82" s="4">
         <v>300</v>
@@ -3951,7 +3951,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L82" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3963,7 +3963,7 @@
         <v>60</v>
       </c>
       <c r="C83" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D83" s="4">
         <v>300</v>
@@ -3989,7 +3989,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L83" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4000,8 +4000,8 @@
       <c r="B84" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C84" s="4">
-        <v>81</v>
+      <c r="C84" s="5">
+        <v>82</v>
       </c>
       <c r="D84" s="4">
         <v>300</v>
@@ -4027,7 +4027,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L84" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4038,8 +4038,8 @@
       <c r="B85" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C85" s="5">
-        <v>82</v>
+      <c r="C85" s="4">
+        <v>83</v>
       </c>
       <c r="D85" s="4">
         <v>300</v>
@@ -4065,7 +4065,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4077,7 +4077,7 @@
         <v>60</v>
       </c>
       <c r="C86" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D86" s="4">
         <v>300</v>
@@ -4103,7 +4103,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L86" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4115,7 +4115,7 @@
         <v>60</v>
       </c>
       <c r="C87" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D87" s="4">
         <v>300</v>
@@ -4126,7 +4126,9 @@
       <c r="F87" s="4">
         <v>70</v>
       </c>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="H87" s="4"/>
       <c r="I87" s="4">
         <f t="shared" si="8"/>
@@ -4141,7 +4143,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L87" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4150,23 +4152,21 @@
         <v>Green</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C88" s="4">
-        <v>85</v>
+        <v>71</v>
+      </c>
+      <c r="C88" s="5">
+        <v>86</v>
       </c>
       <c r="D88" s="4">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E88" s="4">
         <v>0</v>
       </c>
       <c r="F88" s="4">
-        <v>70</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4">
         <f t="shared" si="8"/>
@@ -4178,10 +4178,10 @@
       </c>
       <c r="K88" s="6">
         <f t="shared" si="9"/>
-        <v>15.428571428571431</v>
-      </c>
-      <c r="L88" s="7" t="s">
-        <v>70</v>
+        <v>14.399999999999999</v>
+      </c>
+      <c r="L88" s="7">
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4192,11 +4192,11 @@
       <c r="B89" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C89" s="5">
-        <v>86</v>
+      <c r="C89" s="4">
+        <v>87</v>
       </c>
       <c r="D89" s="4">
-        <v>100</v>
+        <v>86.6</v>
       </c>
       <c r="E89" s="4">
         <v>0</v>
@@ -4216,13 +4216,13 @@
       </c>
       <c r="K89" s="6">
         <f t="shared" si="9"/>
-        <v>14.399999999999999</v>
+        <v>12.470399999999998</v>
       </c>
       <c r="L89" s="7">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
@@ -4231,10 +4231,10 @@
         <v>71</v>
       </c>
       <c r="C90" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D90" s="4">
-        <v>86.6</v>
+        <v>100</v>
       </c>
       <c r="E90" s="4">
         <v>0</v>
@@ -4242,8 +4242,12 @@
       <c r="F90" s="4">
         <v>25</v>
       </c>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
+      <c r="G90" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I90" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4254,52 +4258,48 @@
       </c>
       <c r="K90" s="6">
         <f t="shared" si="9"/>
-        <v>12.470399999999998</v>
+        <v>14.399999999999999</v>
       </c>
       <c r="L90" s="7">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C91" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D91" s="4">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E91" s="4">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="F91" s="4">
         <v>25</v>
       </c>
-      <c r="G91" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
       <c r="I91" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-0.375</v>
       </c>
       <c r="J91" s="4">
         <f t="shared" si="10"/>
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
       <c r="K91" s="6">
         <f t="shared" si="9"/>
-        <v>14.399999999999999</v>
+        <v>10.799999999999999</v>
       </c>
       <c r="L91" s="7">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4310,14 +4310,14 @@
       <c r="B92" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C92" s="4">
-        <v>89</v>
+      <c r="C92" s="5">
+        <v>90</v>
       </c>
       <c r="D92" s="4">
         <v>75</v>
       </c>
       <c r="E92" s="4">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="F92" s="4">
         <v>25</v>
@@ -4326,18 +4326,18 @@
       <c r="H92" s="4"/>
       <c r="I92" s="4">
         <f t="shared" si="8"/>
-        <v>-0.375</v>
+        <v>-0.75</v>
       </c>
       <c r="J92" s="4">
         <f t="shared" si="10"/>
-        <v>0.125</v>
+        <v>-0.625</v>
       </c>
       <c r="K92" s="6">
         <f t="shared" si="9"/>
         <v>10.799999999999999</v>
       </c>
       <c r="L92" s="7">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4348,14 +4348,14 @@
       <c r="B93" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C93" s="5">
-        <v>90</v>
+      <c r="C93" s="4">
+        <v>91</v>
       </c>
       <c r="D93" s="4">
         <v>75</v>
       </c>
       <c r="E93" s="4">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F93" s="4">
         <v>25</v>
@@ -4364,18 +4364,18 @@
       <c r="H93" s="4"/>
       <c r="I93" s="4">
         <f t="shared" si="8"/>
-        <v>-0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="J93" s="4">
         <f t="shared" si="10"/>
-        <v>-0.625</v>
+        <v>-2.125</v>
       </c>
       <c r="K93" s="6">
         <f t="shared" si="9"/>
         <v>10.799999999999999</v>
       </c>
       <c r="L93" s="7">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4387,13 +4387,13 @@
         <v>73</v>
       </c>
       <c r="C94" s="4">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D94" s="4">
         <v>75</v>
       </c>
       <c r="E94" s="4">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F94" s="4">
         <v>25</v>
@@ -4402,7 +4402,7 @@
       <c r="H94" s="4"/>
       <c r="I94" s="4">
         <f t="shared" si="8"/>
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="J94" s="4">
         <f t="shared" si="10"/>
@@ -4413,7 +4413,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="L94" s="7">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4425,13 +4425,13 @@
         <v>73</v>
       </c>
       <c r="C95" s="4">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D95" s="4">
         <v>75</v>
       </c>
       <c r="E95" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F95" s="4">
         <v>25</v>
@@ -4440,18 +4440,18 @@
       <c r="H95" s="4"/>
       <c r="I95" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J95" s="4">
         <f t="shared" si="10"/>
-        <v>-2.125</v>
+        <v>-0.625</v>
       </c>
       <c r="K95" s="6">
         <f t="shared" si="9"/>
         <v>10.799999999999999</v>
       </c>
       <c r="L95" s="7">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4462,14 +4462,14 @@
       <c r="B96" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C96" s="4">
-        <v>93</v>
+      <c r="C96" s="5">
+        <v>94</v>
       </c>
       <c r="D96" s="4">
         <v>75</v>
       </c>
       <c r="E96" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F96" s="4">
         <v>25</v>
@@ -4478,18 +4478,18 @@
       <c r="H96" s="4"/>
       <c r="I96" s="4">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="J96" s="4">
         <f t="shared" si="10"/>
-        <v>-0.625</v>
+        <v>0.125</v>
       </c>
       <c r="K96" s="6">
         <f t="shared" si="9"/>
         <v>10.799999999999999</v>
       </c>
       <c r="L96" s="7">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4500,14 +4500,14 @@
       <c r="B97" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C97" s="5">
-        <v>94</v>
+      <c r="C97" s="4">
+        <v>95</v>
       </c>
       <c r="D97" s="4">
         <v>75</v>
       </c>
       <c r="E97" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F97" s="4">
         <v>25</v>
@@ -4516,21 +4516,21 @@
       <c r="H97" s="4"/>
       <c r="I97" s="4">
         <f t="shared" si="8"/>
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="J97" s="4">
         <f t="shared" si="10"/>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="K97" s="6">
         <f t="shared" si="9"/>
         <v>10.799999999999999</v>
       </c>
       <c r="L97" s="7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
@@ -4539,22 +4539,26 @@
         <v>73</v>
       </c>
       <c r="C98" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D98" s="4">
         <v>75</v>
       </c>
       <c r="E98" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F98" s="4">
         <v>25</v>
       </c>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
+      <c r="G98" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I98" s="4">
         <f t="shared" si="8"/>
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="J98" s="4">
         <f t="shared" si="10"/>
@@ -4565,10 +4569,10 @@
         <v>10.799999999999999</v>
       </c>
       <c r="L98" s="7">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="str">
         <f t="shared" si="11"/>
         <v>Green</v>
@@ -4577,7 +4581,7 @@
         <v>73</v>
       </c>
       <c r="C99" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D99" s="4">
         <v>75</v>
@@ -4588,14 +4592,10 @@
       <c r="F99" s="4">
         <v>25</v>
       </c>
-      <c r="G99" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
       <c r="I99" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="I99:I130" si="12">E99*D99/100</f>
         <v>0</v>
       </c>
       <c r="J99" s="4">
@@ -4603,11 +4603,11 @@
         <v>0.5</v>
       </c>
       <c r="K99" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="K99:K130" si="13">D99*(1/(F99*1000/(60*60)))</f>
         <v>10.799999999999999</v>
       </c>
       <c r="L99" s="7">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4616,10 +4616,10 @@
         <v>Green</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C100" s="4">
-        <v>97</v>
+        <v>75</v>
+      </c>
+      <c r="C100" s="5">
+        <v>98</v>
       </c>
       <c r="D100" s="4">
         <v>75</v>
@@ -4633,19 +4633,19 @@
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4">
-        <f t="shared" ref="I100:I131" si="12">E100*D100/100</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J100" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="J100:J131" si="14">I100+J99</f>
         <v>0.5</v>
       </c>
       <c r="K100" s="6">
-        <f t="shared" ref="K100:K131" si="13">D100*(1/(F100*1000/(60*60)))</f>
+        <f t="shared" si="13"/>
         <v>10.799999999999999</v>
       </c>
       <c r="L100" s="7">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4656,8 +4656,8 @@
       <c r="B101" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C101" s="5">
-        <v>98</v>
+      <c r="C101" s="4">
+        <v>99</v>
       </c>
       <c r="D101" s="4">
         <v>75</v>
@@ -4675,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="J101" s="4">
-        <f t="shared" ref="J101:J132" si="14">I101+J100</f>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="K101" s="6">
@@ -4683,7 +4683,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="L101" s="7">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4695,7 +4695,7 @@
         <v>75</v>
       </c>
       <c r="C102" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D102" s="4">
         <v>75</v>
@@ -4721,7 +4721,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="L102" s="7">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4730,19 +4730,19 @@
         <v>Green</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C103" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D103" s="4">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="E103" s="4">
         <v>0</v>
       </c>
       <c r="F103" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
@@ -4756,31 +4756,31 @@
       </c>
       <c r="K103" s="6">
         <f t="shared" si="13"/>
-        <v>10.799999999999999</v>
+        <v>4.8461538461538467</v>
       </c>
       <c r="L103" s="7">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="A104:A135" si="15">A103</f>
         <v>Green</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C104" s="4">
-        <v>101</v>
+        <v>77</v>
+      </c>
+      <c r="C104" s="5">
+        <v>102</v>
       </c>
       <c r="D104" s="4">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="E104" s="4">
         <v>0</v>
       </c>
       <c r="F104" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -4794,22 +4794,22 @@
       </c>
       <c r="K104" s="6">
         <f t="shared" si="13"/>
-        <v>4.8461538461538467</v>
+        <v>12.857142857142859</v>
       </c>
       <c r="L104" s="7">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="str">
-        <f t="shared" ref="A105:A136" si="15">A104</f>
+        <f t="shared" si="15"/>
         <v>Green</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C105" s="5">
-        <v>102</v>
+      <c r="C105" s="4">
+        <v>103</v>
       </c>
       <c r="D105" s="4">
         <v>100</v>
@@ -4835,7 +4835,7 @@
         <v>12.857142857142859</v>
       </c>
       <c r="L105" s="7">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4847,10 +4847,10 @@
         <v>77</v>
       </c>
       <c r="C106" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D106" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E106" s="4">
         <v>0</v>
@@ -4870,25 +4870,25 @@
       </c>
       <c r="K106" s="6">
         <f t="shared" si="13"/>
-        <v>12.857142857142859</v>
+        <v>10.285714285714286</v>
       </c>
       <c r="L106" s="7">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C107" s="4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D107" s="4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E107" s="4">
         <v>0</v>
@@ -4896,8 +4896,13 @@
       <c r="F107" s="4">
         <v>28</v>
       </c>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
+      <c r="G107" s="8" t="str">
+        <f>G75</f>
+        <v>STATION; DORMONT</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I107" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4908,13 +4913,13 @@
       </c>
       <c r="K107" s="6">
         <f t="shared" si="13"/>
-        <v>10.285714285714286</v>
+        <v>12.857142857142859</v>
       </c>
       <c r="L107" s="7">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -4922,8 +4927,8 @@
       <c r="B108" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C108" s="4">
-        <v>105</v>
+      <c r="C108" s="5">
+        <v>106</v>
       </c>
       <c r="D108" s="4">
         <v>100</v>
@@ -4934,13 +4939,8 @@
       <c r="F108" s="4">
         <v>28</v>
       </c>
-      <c r="G108" s="8" t="str">
-        <f>G76</f>
-        <v>STATION; DORMONT</v>
-      </c>
-      <c r="H108" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
       <c r="I108" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4954,7 +4954,7 @@
         <v>12.857142857142859</v>
       </c>
       <c r="L108" s="7">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4965,11 +4965,11 @@
       <c r="B109" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C109" s="5">
-        <v>106</v>
+      <c r="C109" s="4">
+        <v>107</v>
       </c>
       <c r="D109" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E109" s="4">
         <v>0</v>
@@ -4989,10 +4989,10 @@
       </c>
       <c r="K109" s="6">
         <f t="shared" si="13"/>
-        <v>12.857142857142859</v>
+        <v>11.571428571428573</v>
       </c>
       <c r="L109" s="7">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5004,10 +5004,10 @@
         <v>78</v>
       </c>
       <c r="C110" s="4">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D110" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E110" s="4">
         <v>0</v>
@@ -5015,7 +5015,9 @@
       <c r="F110" s="4">
         <v>28</v>
       </c>
-      <c r="G110" s="4"/>
+      <c r="G110" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="H110" s="4"/>
       <c r="I110" s="4">
         <f t="shared" si="12"/>
@@ -5027,10 +5029,10 @@
       </c>
       <c r="K110" s="6">
         <f t="shared" si="13"/>
-        <v>11.571428571428573</v>
+        <v>12.857142857142859</v>
       </c>
       <c r="L110" s="7">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5042,7 +5044,7 @@
         <v>78</v>
       </c>
       <c r="C111" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D111" s="4">
         <v>100</v>
@@ -5053,9 +5055,7 @@
       <c r="F111" s="4">
         <v>28</v>
       </c>
-      <c r="G111" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4">
         <f t="shared" si="12"/>
@@ -5070,7 +5070,7 @@
         <v>12.857142857142859</v>
       </c>
       <c r="L111" s="7">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5079,10 +5079,10 @@
         <v>Green</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C112" s="4">
-        <v>109</v>
+        <v>79</v>
+      </c>
+      <c r="C112" s="5">
+        <v>110</v>
       </c>
       <c r="D112" s="4">
         <v>100</v>
@@ -5091,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="F112" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
@@ -5105,10 +5105,10 @@
       </c>
       <c r="K112" s="6">
         <f t="shared" si="13"/>
-        <v>12.857142857142859</v>
+        <v>12</v>
       </c>
       <c r="L112" s="7">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5119,8 +5119,8 @@
       <c r="B113" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C113" s="5">
-        <v>110</v>
+      <c r="C113" s="4">
+        <v>111</v>
       </c>
       <c r="D113" s="4">
         <v>100</v>
@@ -5146,7 +5146,7 @@
         <v>12</v>
       </c>
       <c r="L113" s="7">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5158,7 +5158,7 @@
         <v>79</v>
       </c>
       <c r="C114" s="4">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D114" s="4">
         <v>100</v>
@@ -5184,7 +5184,7 @@
         <v>12</v>
       </c>
       <c r="L114" s="7">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5196,7 +5196,7 @@
         <v>79</v>
       </c>
       <c r="C115" s="4">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D115" s="4">
         <v>100</v>
@@ -5222,10 +5222,10 @@
         <v>12</v>
       </c>
       <c r="L115" s="7">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5233,11 +5233,12 @@
       <c r="B116" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C116" s="4">
-        <v>113</v>
+      <c r="C116" s="5">
+        <v>114</v>
       </c>
       <c r="D116" s="4">
-        <v>100</v>
+        <f>100+62</f>
+        <v>162</v>
       </c>
       <c r="E116" s="4">
         <v>0</v>
@@ -5245,8 +5246,13 @@
       <c r="F116" s="4">
         <v>30</v>
       </c>
-      <c r="G116" s="4"/>
-      <c r="H116" s="4"/>
+      <c r="G116" s="8" t="str">
+        <f>G67</f>
+        <v>STATION; GLENBURY</v>
+      </c>
+      <c r="H116" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I116" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5257,13 +5263,13 @@
       </c>
       <c r="K116" s="6">
         <f t="shared" si="13"/>
-        <v>12</v>
+        <v>19.439999999999998</v>
       </c>
       <c r="L116" s="7">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5271,12 +5277,11 @@
       <c r="B117" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C117" s="5">
-        <v>114</v>
+      <c r="C117" s="4">
+        <v>115</v>
       </c>
       <c r="D117" s="4">
-        <f>100+62</f>
-        <v>162</v>
+        <v>100</v>
       </c>
       <c r="E117" s="4">
         <v>0</v>
@@ -5284,13 +5289,8 @@
       <c r="F117" s="4">
         <v>30</v>
       </c>
-      <c r="G117" s="8" t="str">
-        <f>G68</f>
-        <v>STATION; GLENBURY</v>
-      </c>
-      <c r="H117" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
       <c r="I117" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5301,10 +5301,10 @@
       </c>
       <c r="K117" s="6">
         <f t="shared" si="13"/>
-        <v>19.439999999999998</v>
+        <v>12</v>
       </c>
       <c r="L117" s="7">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5316,7 +5316,7 @@
         <v>79</v>
       </c>
       <c r="C118" s="4">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D118" s="4">
         <v>100</v>
@@ -5342,7 +5342,7 @@
         <v>12</v>
       </c>
       <c r="L118" s="7">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5351,19 +5351,19 @@
         <v>Green</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C119" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D119" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E119" s="4">
         <v>0</v>
       </c>
       <c r="F119" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
@@ -5380,7 +5380,7 @@
         <v>12</v>
       </c>
       <c r="L119" s="7">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5391,8 +5391,8 @@
       <c r="B120" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C120" s="4">
-        <v>117</v>
+      <c r="C120" s="5">
+        <v>118</v>
       </c>
       <c r="D120" s="4">
         <v>50</v>
@@ -5418,7 +5418,7 @@
         <v>12</v>
       </c>
       <c r="L120" s="7">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5429,11 +5429,11 @@
       <c r="B121" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C121" s="5">
-        <v>118</v>
+      <c r="C121" s="4">
+        <v>119</v>
       </c>
       <c r="D121" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E121" s="4">
         <v>0</v>
@@ -5453,13 +5453,13 @@
       </c>
       <c r="K121" s="6">
         <f t="shared" si="13"/>
-        <v>12</v>
+        <v>9.6</v>
       </c>
       <c r="L121" s="7">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5468,10 +5468,10 @@
         <v>80</v>
       </c>
       <c r="C122" s="4">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D122" s="4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E122" s="4">
         <v>0</v>
@@ -5491,13 +5491,13 @@
       </c>
       <c r="K122" s="6">
         <f t="shared" si="13"/>
-        <v>9.6</v>
+        <v>12</v>
       </c>
       <c r="L122" s="7">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5506,7 +5506,7 @@
         <v>80</v>
       </c>
       <c r="C123" s="4">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D123" s="4">
         <v>50</v>
@@ -5532,19 +5532,19 @@
         <v>12</v>
       </c>
       <c r="L123" s="7">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" ht="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C124" s="4">
-        <v>121</v>
+        <v>81</v>
+      </c>
+      <c r="C124" s="5">
+        <v>122</v>
       </c>
       <c r="D124" s="4">
         <v>50</v>
@@ -5553,9 +5553,11 @@
         <v>0</v>
       </c>
       <c r="F124" s="4">
-        <v>15</v>
-      </c>
-      <c r="G124" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="H124" s="4"/>
       <c r="I124" s="4">
         <f t="shared" si="12"/>
@@ -5567,13 +5569,13 @@
       </c>
       <c r="K124" s="6">
         <f t="shared" si="13"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L124" s="7">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5581,8 +5583,8 @@
       <c r="B125" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C125" s="5">
-        <v>122</v>
+      <c r="C125" s="4">
+        <v>123</v>
       </c>
       <c r="D125" s="4">
         <v>50</v>
@@ -5593,10 +5595,13 @@
       <c r="F125" s="4">
         <v>20</v>
       </c>
-      <c r="G125" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H125" s="4"/>
+      <c r="G125" s="8" t="str">
+        <f>G59</f>
+        <v>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-YARD)</v>
+      </c>
+      <c r="H125" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I125" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5610,10 +5615,10 @@
         <v>9</v>
       </c>
       <c r="L125" s="7">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5622,7 +5627,7 @@
         <v>81</v>
       </c>
       <c r="C126" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D126" s="4">
         <v>50</v>
@@ -5633,13 +5638,10 @@
       <c r="F126" s="4">
         <v>20</v>
       </c>
-      <c r="G126" s="8" t="str">
-        <f>G60</f>
-        <v>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-YARD)</v>
-      </c>
-      <c r="H126" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G126" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H126" s="4"/>
       <c r="I126" s="4">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5653,7 +5655,7 @@
         <v>9</v>
       </c>
       <c r="L126" s="7">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5665,7 +5667,7 @@
         <v>81</v>
       </c>
       <c r="C127" s="4">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D127" s="4">
         <v>50</v>
@@ -5693,7 +5695,7 @@
         <v>9</v>
       </c>
       <c r="L127" s="7">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5704,8 +5706,8 @@
       <c r="B128" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C128" s="4">
-        <v>125</v>
+      <c r="C128" s="5">
+        <v>126</v>
       </c>
       <c r="D128" s="4">
         <v>50</v>
@@ -5733,7 +5735,7 @@
         <v>9</v>
       </c>
       <c r="L128" s="7">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5744,8 +5746,8 @@
       <c r="B129" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C129" s="5">
-        <v>126</v>
+      <c r="C129" s="4">
+        <v>127</v>
       </c>
       <c r="D129" s="4">
         <v>50</v>
@@ -5773,7 +5775,7 @@
         <v>9</v>
       </c>
       <c r="L129" s="7">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5785,7 +5787,7 @@
         <v>81</v>
       </c>
       <c r="C130" s="4">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D130" s="4">
         <v>50</v>
@@ -5813,7 +5815,7 @@
         <v>9</v>
       </c>
       <c r="L130" s="7">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5825,7 +5827,7 @@
         <v>81</v>
       </c>
       <c r="C131" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D131" s="4">
         <v>50</v>
@@ -5841,7 +5843,7 @@
       </c>
       <c r="H131" s="4"/>
       <c r="I131" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="I131:I152" si="16">E131*D131/100</f>
         <v>0</v>
       </c>
       <c r="J131" s="4">
@@ -5849,11 +5851,11 @@
         <v>0.5</v>
       </c>
       <c r="K131" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="K131:K152" si="17">D131*(1/(F131*1000/(60*60)))</f>
         <v>9</v>
       </c>
       <c r="L131" s="7">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5864,8 +5866,8 @@
       <c r="B132" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C132" s="4">
-        <v>129</v>
+      <c r="C132" s="5">
+        <v>130</v>
       </c>
       <c r="D132" s="4">
         <v>50</v>
@@ -5881,19 +5883,19 @@
       </c>
       <c r="H132" s="4"/>
       <c r="I132" s="4">
-        <f t="shared" ref="I132:I153" si="16">E132*D132/100</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J132" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="J132:J152" si="18">I132+J131</f>
         <v>0.5</v>
       </c>
       <c r="K132" s="6">
-        <f t="shared" ref="K132:K153" si="17">D132*(1/(F132*1000/(60*60)))</f>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="L132" s="7">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5904,8 +5906,8 @@
       <c r="B133" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C133" s="5">
-        <v>130</v>
+      <c r="C133" s="4">
+        <v>131</v>
       </c>
       <c r="D133" s="4">
         <v>50</v>
@@ -5925,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="J133" s="4">
-        <f t="shared" ref="J133:J164" si="18">I133+J132</f>
+        <f t="shared" si="18"/>
         <v>0.5</v>
       </c>
       <c r="K133" s="6">
@@ -5933,10 +5935,10 @@
         <v>9</v>
       </c>
       <c r="L133" s="7">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5945,7 +5947,7 @@
         <v>81</v>
       </c>
       <c r="C134" s="4">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D134" s="4">
         <v>50</v>
@@ -5956,10 +5958,13 @@
       <c r="F134" s="4">
         <v>20</v>
       </c>
-      <c r="G134" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H134" s="4"/>
+      <c r="G134" s="8" t="str">
+        <f>G50</f>
+        <v>STATION; INGLEWOOD; UNDERGROUND</v>
+      </c>
+      <c r="H134" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I134" s="4">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -5973,10 +5978,10 @@
         <v>9</v>
       </c>
       <c r="L134" s="7">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="str">
         <f t="shared" si="15"/>
         <v>Green</v>
@@ -5985,7 +5990,7 @@
         <v>81</v>
       </c>
       <c r="C135" s="4">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D135" s="4">
         <v>50</v>
@@ -5996,13 +6001,10 @@
       <c r="F135" s="4">
         <v>20</v>
       </c>
-      <c r="G135" s="8" t="str">
-        <f>G51</f>
-        <v>STATION; INGLEWOOD; UNDERGROUND</v>
-      </c>
-      <c r="H135" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G135" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H135" s="4"/>
       <c r="I135" s="4">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -6016,19 +6018,19 @@
         <v>9</v>
       </c>
       <c r="L135" s="7">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="A136:A152" si="19">A135</f>
         <v>Green</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C136" s="4">
-        <v>133</v>
+      <c r="C136" s="5">
+        <v>134</v>
       </c>
       <c r="D136" s="4">
         <v>50</v>
@@ -6056,19 +6058,19 @@
         <v>9</v>
       </c>
       <c r="L136" s="7">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="str">
-        <f t="shared" ref="A137:A153" si="19">A136</f>
+        <f t="shared" si="19"/>
         <v>Green</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C137" s="5">
-        <v>134</v>
+      <c r="C137" s="4">
+        <v>135</v>
       </c>
       <c r="D137" s="4">
         <v>50</v>
@@ -6096,7 +6098,7 @@
         <v>9</v>
       </c>
       <c r="L137" s="7">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6108,7 +6110,7 @@
         <v>81</v>
       </c>
       <c r="C138" s="4">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D138" s="4">
         <v>50</v>
@@ -6136,7 +6138,7 @@
         <v>9</v>
       </c>
       <c r="L138" s="7">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6148,7 +6150,7 @@
         <v>81</v>
       </c>
       <c r="C139" s="4">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D139" s="4">
         <v>50</v>
@@ -6176,7 +6178,7 @@
         <v>9</v>
       </c>
       <c r="L139" s="7">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6187,8 +6189,8 @@
       <c r="B140" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C140" s="4">
-        <v>137</v>
+      <c r="C140" s="5">
+        <v>138</v>
       </c>
       <c r="D140" s="4">
         <v>50</v>
@@ -6216,7 +6218,7 @@
         <v>9</v>
       </c>
       <c r="L140" s="7">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6227,8 +6229,8 @@
       <c r="B141" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C141" s="5">
-        <v>138</v>
+      <c r="C141" s="4">
+        <v>139</v>
       </c>
       <c r="D141" s="4">
         <v>50</v>
@@ -6256,7 +6258,7 @@
         <v>9</v>
       </c>
       <c r="L141" s="7">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6268,7 +6270,7 @@
         <v>81</v>
       </c>
       <c r="C142" s="4">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D142" s="4">
         <v>50</v>
@@ -6296,10 +6298,10 @@
         <v>9</v>
       </c>
       <c r="L142" s="7">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="str">
         <f t="shared" si="19"/>
         <v>Green</v>
@@ -6308,7 +6310,7 @@
         <v>81</v>
       </c>
       <c r="C143" s="4">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D143" s="4">
         <v>50</v>
@@ -6319,10 +6321,13 @@
       <c r="F143" s="4">
         <v>20</v>
       </c>
-      <c r="G143" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H143" s="4"/>
+      <c r="G143" s="8" t="str">
+        <f>G41</f>
+        <v>STATION; CENTRAL; UNDERDROUND</v>
+      </c>
+      <c r="H143" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I143" s="4">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -6336,10 +6341,10 @@
         <v>9</v>
       </c>
       <c r="L143" s="7">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="str">
         <f t="shared" si="19"/>
         <v>Green</v>
@@ -6347,8 +6352,8 @@
       <c r="B144" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C144" s="4">
-        <v>141</v>
+      <c r="C144" s="5">
+        <v>142</v>
       </c>
       <c r="D144" s="4">
         <v>50</v>
@@ -6359,13 +6364,10 @@
       <c r="F144" s="4">
         <v>20</v>
       </c>
-      <c r="G144" s="8" t="str">
-        <f>G42</f>
-        <v>STATION; CENTRAL; UNDERDROUND</v>
-      </c>
-      <c r="H144" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G144" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H144" s="4"/>
       <c r="I144" s="4">
         <f t="shared" si="16"/>
         <v>0</v>
@@ -6379,7 +6381,7 @@
         <v>9</v>
       </c>
       <c r="L144" s="7">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6390,8 +6392,8 @@
       <c r="B145" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C145" s="5">
-        <v>142</v>
+      <c r="C145" s="4">
+        <v>143</v>
       </c>
       <c r="D145" s="4">
         <v>50</v>
@@ -6419,7 +6421,7 @@
         <v>9</v>
       </c>
       <c r="L145" s="7">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6428,10 +6430,10 @@
         <v>Green</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C146" s="4">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D146" s="4">
         <v>50</v>
@@ -6442,9 +6444,7 @@
       <c r="F146" s="4">
         <v>20</v>
       </c>
-      <c r="G146" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4">
         <f t="shared" si="16"/>
@@ -6459,7 +6459,7 @@
         <v>9</v>
       </c>
       <c r="L146" s="7">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6471,7 +6471,7 @@
         <v>82</v>
       </c>
       <c r="C147" s="4">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D147" s="4">
         <v>50</v>
@@ -6497,7 +6497,7 @@
         <v>9</v>
       </c>
       <c r="L147" s="7">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6508,8 +6508,8 @@
       <c r="B148" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C148" s="4">
-        <v>145</v>
+      <c r="C148" s="5">
+        <v>146</v>
       </c>
       <c r="D148" s="4">
         <v>50</v>
@@ -6535,7 +6535,7 @@
         <v>9</v>
       </c>
       <c r="L148" s="7">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="149" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6544,10 +6544,10 @@
         <v>Green</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C149" s="5">
-        <v>146</v>
+        <v>83</v>
+      </c>
+      <c r="C149" s="4">
+        <v>147</v>
       </c>
       <c r="D149" s="4">
         <v>50</v>
@@ -6573,7 +6573,7 @@
         <v>9</v>
       </c>
       <c r="L149" s="7">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6585,10 +6585,11 @@
         <v>83</v>
       </c>
       <c r="C150" s="4">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D150" s="4">
-        <v>50</v>
+        <f>40+144</f>
+        <v>184</v>
       </c>
       <c r="E150" s="4">
         <v>0</v>
@@ -6608,10 +6609,10 @@
       </c>
       <c r="K150" s="6">
         <f t="shared" si="17"/>
-        <v>9</v>
+        <v>33.119999999999997</v>
       </c>
       <c r="L150" s="7">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6623,11 +6624,10 @@
         <v>83</v>
       </c>
       <c r="C151" s="4">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D151" s="4">
-        <f>40+144</f>
-        <v>184</v>
+        <v>40</v>
       </c>
       <c r="E151" s="4">
         <v>0</v>
@@ -6647,10 +6647,10 @@
       </c>
       <c r="K151" s="6">
         <f t="shared" si="17"/>
-        <v>33.119999999999997</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="L151" s="7">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6659,13 +6659,13 @@
         <v>Green</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C152" s="4">
-        <v>149</v>
+        <v>84</v>
+      </c>
+      <c r="C152" s="5">
+        <v>150</v>
       </c>
       <c r="D152" s="4">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E152" s="4">
         <v>0</v>
@@ -6685,48 +6685,48 @@
       </c>
       <c r="K152" s="6">
         <f t="shared" si="17"/>
-        <v>7.1999999999999993</v>
+        <v>6.3</v>
       </c>
       <c r="L152" s="7">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f>A8</f>
         <v>Green</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C153" s="5">
-        <v>150</v>
+        <v>17</v>
+      </c>
+      <c r="C153" s="4">
+        <v>151</v>
       </c>
       <c r="D153" s="4">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E153" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F153" s="4">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f>E153*D153/100</f>
+        <v>2.5</v>
       </c>
       <c r="J153" s="4">
-        <f t="shared" si="18"/>
-        <v>0.5</v>
+        <f>I153+J8</f>
+        <v>14.5</v>
       </c>
       <c r="K153" s="6">
-        <f t="shared" si="17"/>
-        <v>6.3</v>
+        <f>D153*(1/(F153*1000/(60*60)))</f>
+        <v>4</v>
       </c>
       <c r="L153" s="7">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -6785,20 +6785,6 @@
       <c r="K157" s="7"/>
       <c r="L157" s="7"/>
     </row>
-    <row r="158" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A158" s="4"/>
-      <c r="B158" s="4"/>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4"/>
-      <c r="E158" s="4"/>
-      <c r="F158" s="4"/>
-      <c r="G158" s="4"/>
-      <c r="H158" s="4"/>
-      <c r="I158" s="7"/>
-      <c r="J158" s="7"/>
-      <c r="K158" s="7"/>
-      <c r="L158" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
fixed station name recognition, added auto-manual toggle to ui
</commit_message>
<xml_diff>
--- a/CTC_Office/Green_Line_Layout.xlsx
+++ b/CTC_Office/Green_Line_Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaseckrich/Documents/Classes/ECE 1140/ECE1140_TermProject/CTC_Office/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0544D6C0-E35D-9A4E-A9FB-64C917A9AA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC81195-6BBA-B947-838D-3AF0DB916936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="28300" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>STATION; PIONEER</t>
-  </si>
-  <si>
     <t>Left</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>STATION; EDGEBROOK</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>14, 16</t>
   </si>
   <si>
-    <t>STATION</t>
-  </si>
-  <si>
     <t>Left/Right</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
     <t>20, 22</t>
   </si>
   <si>
-    <t>STATION; WHITED</t>
-  </si>
-  <si>
     <t>21, 23</t>
   </si>
   <si>
@@ -173,9 +161,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>STATION; SOUTH BANK</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -206,15 +191,9 @@
     <t>SWITCH FROM YARD (Yard-63)</t>
   </si>
   <si>
-    <t>STATION; GLENBURY</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>STATION; DORMONT</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -257,15 +236,9 @@
     <t>O</t>
   </si>
   <si>
-    <t>STATION; POPLAR</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>STATION;   CASTLE SHANNON</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -294,6 +267,33 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>STATION; PIONEER;</t>
+  </si>
+  <si>
+    <t>STATION; EDGEBROOK;</t>
+  </si>
+  <si>
+    <t>STATION; MONROEVILLE;</t>
+  </si>
+  <si>
+    <t>STATION; WHITED;</t>
+  </si>
+  <si>
+    <t>STATION; SOUTH BANK;</t>
+  </si>
+  <si>
+    <t>STATION; GLENBURY;</t>
+  </si>
+  <si>
+    <t>STATION; DORMONT;</t>
+  </si>
+  <si>
+    <t>STATION; POPLAR;</t>
+  </si>
+  <si>
+    <t>STATION; CASTLE SHANNON;</t>
   </si>
 </sst>
 </file>
@@ -734,8 +734,8 @@
   </sheetPr>
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -789,7 +789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -862,7 +862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f t="shared" ref="A4:A38" si="2">A3</f>
         <v>Green</v>
@@ -883,10 +883,10 @@
         <v>45</v>
       </c>
       <c r="G4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="I4" s="12">
         <f t="shared" si="0"/>
@@ -948,7 +948,7 @@
         <v>Green</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="11">
         <v>4</v>
@@ -986,7 +986,7 @@
         <v>Green</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="12">
         <v>5</v>
@@ -1024,7 +1024,7 @@
         <v>Green</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="12">
         <v>6</v>
@@ -1062,7 +1062,7 @@
         <v>Green</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="11">
         <v>7</v>
@@ -1100,7 +1100,7 @@
         <v>Green</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="12">
         <v>8</v>
@@ -1138,7 +1138,7 @@
         <v>Green</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12">
         <v>9</v>
@@ -1153,10 +1153,10 @@
         <v>45</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="12">
         <f t="shared" si="0"/>
@@ -1180,7 +1180,7 @@
         <v>Green</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="11">
         <v>10</v>
@@ -1218,7 +1218,7 @@
         <v>Green</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="12">
         <v>11</v>
@@ -1256,7 +1256,7 @@
         <v>Green</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="11">
         <v>12</v>
@@ -1293,7 +1293,7 @@
         <v>Green</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="12">
         <v>13</v>
@@ -1308,7 +1308,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="12">
@@ -1324,7 +1324,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,7 +1333,7 @@
         <v>Green</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="12">
         <v>14</v>
@@ -1362,7 +1362,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1371,7 +1371,7 @@
         <v>Green</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="11">
         <v>15</v>
@@ -1400,7 +1400,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L17" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1409,7 +1409,7 @@
         <v>Green</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="12">
         <v>16</v>
@@ -1424,10 +1424,10 @@
         <v>70</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
@@ -1442,7 +1442,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1451,7 +1451,7 @@
         <v>Green</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" s="11">
         <v>17</v>
@@ -1480,7 +1480,7 @@
         <v>9</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1489,7 +1489,7 @@
         <v>Green</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="12">
         <v>18</v>
@@ -1518,7 +1518,7 @@
         <v>9</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1527,7 +1527,7 @@
         <v>Green</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="12">
         <v>19</v>
@@ -1542,7 +1542,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="12">
@@ -1558,7 +1558,7 @@
         <v>9</v>
       </c>
       <c r="L21" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1567,7 +1567,7 @@
         <v>Green</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="11">
         <v>20</v>
@@ -1596,7 +1596,7 @@
         <v>9</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1605,7 +1605,7 @@
         <v>Green</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C23" s="12">
         <v>21</v>
@@ -1634,7 +1634,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1643,7 +1643,7 @@
         <v>Green</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="11">
         <v>22</v>
@@ -1658,10 +1658,10 @@
         <v>70</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I24" s="12">
         <f t="shared" si="0"/>
@@ -1676,16 +1676,16 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" s="12">
         <v>23</v>
@@ -1714,7 +1714,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1723,7 +1723,7 @@
         <v>Green</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C26" s="12">
         <v>24</v>
@@ -1752,7 +1752,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1761,7 +1761,7 @@
         <v>Green</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27" s="11">
         <v>25</v>
@@ -1790,7 +1790,7 @@
         <v>10.285714285714286</v>
       </c>
       <c r="L27" s="18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1799,7 +1799,7 @@
         <v>Green</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28" s="12">
         <v>26</v>
@@ -1828,7 +1828,7 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +1837,7 @@
         <v>Green</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="11">
         <v>27</v>
@@ -1866,16 +1866,16 @@
         <v>6</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C30" s="12">
         <v>28</v>
@@ -1890,7 +1890,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="12">
@@ -1906,7 +1906,7 @@
         <v>6</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1915,7 +1915,7 @@
         <v>Green</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C31" s="12">
         <v>29</v>
@@ -1953,7 +1953,7 @@
         <v>Green</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C32" s="11">
         <v>30</v>
@@ -1985,13 +1985,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" s="12">
         <v>31</v>
@@ -2006,10 +2006,10 @@
         <v>30</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
@@ -2033,7 +2033,7 @@
         <v>Green</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C34" s="11">
         <v>32</v>
@@ -2071,7 +2071,7 @@
         <v>Green</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C35" s="12">
         <v>33</v>
@@ -2109,7 +2109,7 @@
         <v>Green</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C36" s="12">
         <v>34</v>
@@ -2147,7 +2147,7 @@
         <v>Green</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" s="11">
         <v>35</v>
@@ -2185,7 +2185,7 @@
         <v>Green</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C38" s="12">
         <v>36</v>
@@ -2200,7 +2200,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="12">
@@ -2225,7 +2225,7 @@
         <v>Green</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C39" s="12">
         <v>37</v>
@@ -2240,7 +2240,7 @@
         <v>30</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="12">
@@ -2265,7 +2265,7 @@
         <v>Green</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C40" s="11">
         <v>38</v>
@@ -2280,7 +2280,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="12">
@@ -2305,7 +2305,7 @@
         <v>Green</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C41" s="12">
         <v>39</v>
@@ -2320,10 +2320,10 @@
         <v>30</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I41" s="12">
         <f t="shared" si="4"/>
@@ -2347,7 +2347,7 @@
         <v>Green</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C42" s="12">
         <v>40</v>
@@ -2362,7 +2362,7 @@
         <v>30</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="12">
@@ -2387,7 +2387,7 @@
         <v>Green</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C43" s="11">
         <v>41</v>
@@ -2402,7 +2402,7 @@
         <v>30</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="12">
@@ -2427,7 +2427,7 @@
         <v>Green</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C44" s="12">
         <v>42</v>
@@ -2442,7 +2442,7 @@
         <v>30</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="12">
@@ -2467,7 +2467,7 @@
         <v>Green</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C45" s="12">
         <v>43</v>
@@ -2482,7 +2482,7 @@
         <v>30</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="12">
@@ -2507,7 +2507,7 @@
         <v>Green</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C46" s="11">
         <v>44</v>
@@ -2522,7 +2522,7 @@
         <v>30</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="12">
@@ -2547,7 +2547,7 @@
         <v>Green</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C47" s="12">
         <v>45</v>
@@ -2562,7 +2562,7 @@
         <v>30</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="12">
@@ -2587,7 +2587,7 @@
         <v>Green</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C48" s="12">
         <v>46</v>
@@ -2602,7 +2602,7 @@
         <v>30</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="12">
@@ -2627,7 +2627,7 @@
         <v>Green</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C49" s="11">
         <v>47</v>
@@ -2642,7 +2642,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="12">
@@ -2667,7 +2667,7 @@
         <v>Green</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C50" s="12">
         <v>48</v>
@@ -2682,10 +2682,10 @@
         <v>30</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I50" s="12">
         <f t="shared" si="4"/>
@@ -2709,7 +2709,7 @@
         <v>Green</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C51" s="12">
         <v>49</v>
@@ -2724,7 +2724,7 @@
         <v>30</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="12">
@@ -2749,7 +2749,7 @@
         <v>Green</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C52" s="11">
         <v>50</v>
@@ -2764,7 +2764,7 @@
         <v>30</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="12">
@@ -2789,7 +2789,7 @@
         <v>Green</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C53" s="12">
         <v>51</v>
@@ -2804,7 +2804,7 @@
         <v>30</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="12">
@@ -2829,7 +2829,7 @@
         <v>Green</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C54" s="12">
         <v>52</v>
@@ -2844,7 +2844,7 @@
         <v>30</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="12">
@@ -2869,7 +2869,7 @@
         <v>Green</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C55" s="11">
         <v>53</v>
@@ -2884,7 +2884,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="12">
@@ -2909,7 +2909,7 @@
         <v>Green</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C56" s="12">
         <v>54</v>
@@ -2924,7 +2924,7 @@
         <v>30</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="12">
@@ -2949,7 +2949,7 @@
         <v>Green</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C57" s="12">
         <v>55</v>
@@ -2964,7 +2964,7 @@
         <v>30</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="12">
@@ -2989,7 +2989,7 @@
         <v>Green</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C58" s="11">
         <v>56</v>
@@ -3004,7 +3004,7 @@
         <v>30</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="12">
@@ -3023,13 +3023,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C59" s="12">
         <v>57</v>
@@ -3044,10 +3044,10 @@
         <v>30</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I59" s="12">
         <f t="shared" si="4"/>
@@ -3071,7 +3071,7 @@
         <v>Green</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C60" s="12">
         <v>58</v>
@@ -3109,7 +3109,7 @@
         <v>Green</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C61" s="11">
         <v>59</v>
@@ -3147,7 +3147,7 @@
         <v>Green</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C62" s="12">
         <v>60</v>
@@ -3185,7 +3185,7 @@
         <v>Green</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C63" s="12">
         <v>61</v>
@@ -3223,7 +3223,7 @@
         <v>Green</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C64" s="11">
         <v>62</v>
@@ -3254,13 +3254,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C65" s="12">
         <v>63</v>
@@ -3275,7 +3275,7 @@
         <v>70</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H65" s="7"/>
       <c r="I65" s="12">
@@ -3294,13 +3294,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C66" s="12">
         <v>64</v>
@@ -3332,13 +3332,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C67" s="11">
         <v>65</v>
@@ -3353,10 +3353,10 @@
         <v>70</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I67" s="12">
         <f t="shared" ref="I67:I98" si="8">E67*D67/100</f>
@@ -3380,7 +3380,7 @@
         <v>Green</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C68" s="12">
         <v>66</v>
@@ -3418,7 +3418,7 @@
         <v>Green</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C69" s="12">
         <v>67</v>
@@ -3456,7 +3456,7 @@
         <v>Green</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C70" s="11">
         <v>68</v>
@@ -3494,7 +3494,7 @@
         <v>Green</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C71" s="12">
         <v>69</v>
@@ -3532,7 +3532,7 @@
         <v>Green</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C72" s="12">
         <v>70</v>
@@ -3570,7 +3570,7 @@
         <v>Green</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C73" s="11">
         <v>71</v>
@@ -3608,7 +3608,7 @@
         <v>Green</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C74" s="12">
         <v>72</v>
@@ -3646,7 +3646,7 @@
         <v>Green</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C75" s="12">
         <v>73</v>
@@ -3661,10 +3661,10 @@
         <v>40</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I75" s="12">
         <f t="shared" si="8"/>
@@ -3688,7 +3688,7 @@
         <v>Green</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C76" s="11">
         <v>74</v>
@@ -3726,7 +3726,7 @@
         <v>Green</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C77" s="12">
         <v>75</v>
@@ -3764,7 +3764,7 @@
         <v>Green</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C78" s="12">
         <v>76</v>
@@ -3802,7 +3802,7 @@
         <v>Green</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C79" s="12">
         <v>77</v>
@@ -3817,10 +3817,10 @@
         <v>70</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I79" s="12">
         <f t="shared" si="8"/>
@@ -3835,7 +3835,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L79" s="18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3844,7 +3844,7 @@
         <v>Green</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C80" s="11">
         <v>78</v>
@@ -3873,7 +3873,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L80" s="18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3882,7 +3882,7 @@
         <v>Green</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C81" s="12">
         <v>79</v>
@@ -3911,7 +3911,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L81" s="18" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3920,7 +3920,7 @@
         <v>Green</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C82" s="12">
         <v>80</v>
@@ -3949,7 +3949,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L82" s="18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3958,7 +3958,7 @@
         <v>Green</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C83" s="12">
         <v>81</v>
@@ -3987,7 +3987,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L83" s="18" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3996,7 +3996,7 @@
         <v>Green</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C84" s="11">
         <v>82</v>
@@ -4025,7 +4025,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L84" s="18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4034,7 +4034,7 @@
         <v>Green</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C85" s="12">
         <v>83</v>
@@ -4063,7 +4063,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L85" s="18" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4072,7 +4072,7 @@
         <v>Green</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C86" s="12">
         <v>84</v>
@@ -4101,7 +4101,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L86" s="18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4110,7 +4110,7 @@
         <v>Green</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C87" s="12">
         <v>85</v>
@@ -4125,7 +4125,7 @@
         <v>70</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="12">
@@ -4141,7 +4141,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L87" s="18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4150,7 +4150,7 @@
         <v>Green</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C88" s="11">
         <v>86</v>
@@ -4188,7 +4188,7 @@
         <v>Green</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C89" s="12">
         <v>87</v>
@@ -4226,7 +4226,7 @@
         <v>Green</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C90" s="12">
         <v>88</v>
@@ -4241,10 +4241,10 @@
         <v>25</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I90" s="12">
         <f t="shared" si="8"/>
@@ -4268,7 +4268,7 @@
         <v>Green</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C91" s="12">
         <v>89</v>
@@ -4306,7 +4306,7 @@
         <v>Green</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C92" s="11">
         <v>90</v>
@@ -4344,7 +4344,7 @@
         <v>Green</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C93" s="12">
         <v>91</v>
@@ -4382,7 +4382,7 @@
         <v>Green</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C94" s="12">
         <v>92</v>
@@ -4420,7 +4420,7 @@
         <v>Green</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C95" s="12">
         <v>93</v>
@@ -4458,7 +4458,7 @@
         <v>Green</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C96" s="11">
         <v>94</v>
@@ -4496,7 +4496,7 @@
         <v>Green</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C97" s="12">
         <v>95</v>
@@ -4534,7 +4534,7 @@
         <v>Green</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C98" s="12">
         <v>96</v>
@@ -4549,10 +4549,10 @@
         <v>25</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I98" s="12">
         <f t="shared" si="8"/>
@@ -4576,7 +4576,7 @@
         <v>Green</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C99" s="12">
         <v>97</v>
@@ -4614,7 +4614,7 @@
         <v>Green</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C100" s="11">
         <v>98</v>
@@ -4652,7 +4652,7 @@
         <v>Green</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C101" s="12">
         <v>99</v>
@@ -4690,7 +4690,7 @@
         <v>Green</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C102" s="12">
         <v>100</v>
@@ -4728,7 +4728,7 @@
         <v>Green</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C103" s="12">
         <v>101</v>
@@ -4766,7 +4766,7 @@
         <v>Green</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C104" s="11">
         <v>102</v>
@@ -4804,7 +4804,7 @@
         <v>Green</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C105" s="12">
         <v>103</v>
@@ -4842,7 +4842,7 @@
         <v>Green</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C106" s="12">
         <v>104</v>
@@ -4880,7 +4880,7 @@
         <v>Green</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C107" s="12">
         <v>105</v>
@@ -4896,10 +4896,10 @@
       </c>
       <c r="G107" s="15" t="str">
         <f>G75</f>
-        <v>STATION; DORMONT</v>
+        <v>STATION; DORMONT;</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I107" s="12">
         <f t="shared" si="12"/>
@@ -4923,7 +4923,7 @@
         <v>Green</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C108" s="11">
         <v>106</v>
@@ -4961,7 +4961,7 @@
         <v>Green</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C109" s="12">
         <v>107</v>
@@ -4999,7 +4999,7 @@
         <v>Green</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C110" s="12">
         <v>108</v>
@@ -5014,7 +5014,7 @@
         <v>28</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="12">
@@ -5039,7 +5039,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C111" s="12">
         <v>109</v>
@@ -5077,7 +5077,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C112" s="11">
         <v>110</v>
@@ -5115,7 +5115,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C113" s="12">
         <v>111</v>
@@ -5153,7 +5153,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C114" s="12">
         <v>112</v>
@@ -5191,7 +5191,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C115" s="12">
         <v>113</v>
@@ -5229,7 +5229,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C116" s="11">
         <v>114</v>
@@ -5245,10 +5245,10 @@
       </c>
       <c r="G116" s="15" t="str">
         <f>G67</f>
-        <v>STATION; GLENBURY</v>
+        <v>STATION; GLENBURY;</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I116" s="12">
         <f t="shared" si="12"/>
@@ -5272,7 +5272,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C117" s="12">
         <v>115</v>
@@ -5310,7 +5310,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C118" s="12">
         <v>116</v>
@@ -5348,7 +5348,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C119" s="12">
         <v>117</v>
@@ -5386,7 +5386,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C120" s="11">
         <v>118</v>
@@ -5424,7 +5424,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C121" s="12">
         <v>119</v>
@@ -5462,7 +5462,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C122" s="12">
         <v>120</v>
@@ -5500,7 +5500,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C123" s="12">
         <v>121</v>
@@ -5538,7 +5538,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C124" s="11">
         <v>122</v>
@@ -5553,7 +5553,7 @@
         <v>20</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="12">
@@ -5578,7 +5578,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C125" s="12">
         <v>123</v>
@@ -5597,7 +5597,7 @@
         <v>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-YARD)</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I125" s="12">
         <f t="shared" si="12"/>
@@ -5621,7 +5621,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C126" s="12">
         <v>124</v>
@@ -5636,7 +5636,7 @@
         <v>20</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="12">
@@ -5661,7 +5661,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C127" s="12">
         <v>125</v>
@@ -5676,7 +5676,7 @@
         <v>20</v>
       </c>
       <c r="G127" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="12">
@@ -5701,7 +5701,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C128" s="11">
         <v>126</v>
@@ -5716,7 +5716,7 @@
         <v>20</v>
       </c>
       <c r="G128" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="12">
@@ -5741,7 +5741,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C129" s="12">
         <v>127</v>
@@ -5756,7 +5756,7 @@
         <v>20</v>
       </c>
       <c r="G129" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="12">
@@ -5781,7 +5781,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C130" s="12">
         <v>128</v>
@@ -5796,7 +5796,7 @@
         <v>20</v>
       </c>
       <c r="G130" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="12">
@@ -5821,7 +5821,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C131" s="12">
         <v>129</v>
@@ -5836,7 +5836,7 @@
         <v>20</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="12">
@@ -5861,7 +5861,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C132" s="11">
         <v>130</v>
@@ -5876,7 +5876,7 @@
         <v>20</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="12">
@@ -5901,7 +5901,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C133" s="12">
         <v>131</v>
@@ -5916,7 +5916,7 @@
         <v>20</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="12">
@@ -5941,7 +5941,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C134" s="12">
         <v>132</v>
@@ -5960,7 +5960,7 @@
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I134" s="12">
         <f t="shared" si="16"/>
@@ -5984,7 +5984,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C135" s="12">
         <v>133</v>
@@ -5999,7 +5999,7 @@
         <v>20</v>
       </c>
       <c r="G135" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="12">
@@ -6024,7 +6024,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C136" s="11">
         <v>134</v>
@@ -6039,7 +6039,7 @@
         <v>20</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="12">
@@ -6064,7 +6064,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C137" s="12">
         <v>135</v>
@@ -6079,7 +6079,7 @@
         <v>20</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="12">
@@ -6104,7 +6104,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C138" s="12">
         <v>136</v>
@@ -6119,7 +6119,7 @@
         <v>20</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="12">
@@ -6127,7 +6127,7 @@
         <v>0</v>
       </c>
       <c r="J138" s="13">
-        <f t="shared" ref="J138:J169" si="19">I138+J137</f>
+        <f t="shared" ref="J138:J152" si="19">I138+J137</f>
         <v>0.5</v>
       </c>
       <c r="K138" s="14">
@@ -6144,7 +6144,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C139" s="12">
         <v>137</v>
@@ -6159,7 +6159,7 @@
         <v>20</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="12">
@@ -6184,7 +6184,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C140" s="11">
         <v>138</v>
@@ -6199,7 +6199,7 @@
         <v>20</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="12">
@@ -6224,7 +6224,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C141" s="12">
         <v>139</v>
@@ -6239,7 +6239,7 @@
         <v>20</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="12">
@@ -6264,7 +6264,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C142" s="12">
         <v>140</v>
@@ -6279,7 +6279,7 @@
         <v>20</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="12">
@@ -6304,7 +6304,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C143" s="12">
         <v>141</v>
@@ -6323,7 +6323,7 @@
         <v>STATION; CENTRAL; UNDERDROUND</v>
       </c>
       <c r="H143" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I143" s="12">
         <f t="shared" si="16"/>
@@ -6347,7 +6347,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C144" s="11">
         <v>142</v>
@@ -6362,7 +6362,7 @@
         <v>20</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="12">
@@ -6387,7 +6387,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C145" s="12">
         <v>143</v>
@@ -6402,7 +6402,7 @@
         <v>20</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="12">
@@ -6427,7 +6427,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C146" s="12">
         <v>144</v>
@@ -6465,7 +6465,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C147" s="12">
         <v>145</v>
@@ -6503,7 +6503,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C148" s="11">
         <v>146</v>
@@ -6541,7 +6541,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C149" s="12">
         <v>147</v>
@@ -6579,7 +6579,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C150" s="12">
         <v>148</v>
@@ -6618,7 +6618,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C151" s="12">
         <v>149</v>
@@ -6656,7 +6656,7 @@
         <v>Green</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C152" s="11">
         <v>150</v>
@@ -6694,7 +6694,7 @@
         <v>Green</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C153" s="12">
         <v>151</v>

</xml_diff>

<commit_message>
more UI addition. started support for destination list
</commit_message>
<xml_diff>
--- a/CTC_Office/Green_Line_Layout.xlsx
+++ b/CTC_Office/Green_Line_Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaseckrich/Documents/Classes/ECE 1140/ECE1140_TermProject/CTC_Office/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC81195-6BBA-B947-838D-3AF0DB916936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC703ED-CB07-7A44-A88A-5CFA045E4C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   </sheetPr>
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Figured out how to modify simulation speed. Simulated time in CTC matches the selected speedup. Updated the station drop down to account for passing stations twice, either the same block twice or two different blocks connected to the same station. UI updates. Automatic and manual mode change the available controls. Must be in maintenance mode to put block in maintenance.
</commit_message>
<xml_diff>
--- a/CTC_Office/Green_Line_Layout.xlsx
+++ b/CTC_Office/Green_Line_Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaseckrich/Documents/Classes/ECE 1140/ECE1140_TermProject/CTC_Office/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC703ED-CB07-7A44-A88A-5CFA045E4C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8D5055-E2C6-D242-A20D-DEB21857D3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="88">
   <si>
     <t>Line</t>
   </si>
@@ -92,9 +92,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>SWITCH (12-13; 1-13)</t>
-  </si>
-  <si>
     <t>12, 14</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>26, 28</t>
   </si>
   <si>
-    <t>SWITCH (28-29; 150-28)</t>
-  </si>
-  <si>
     <t>27, 29</t>
   </si>
   <si>
@@ -179,18 +173,12 @@
     <t>STATION; INGLEWOOD; UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-YARD)</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
     <t>K</t>
   </si>
   <si>
-    <t>SWITCH FROM YARD (Yard-63)</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -200,9 +188,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>STATION; MT LEBANON;SWITCH (76-77;77-101)</t>
-  </si>
-  <si>
     <t>101, 78</t>
   </si>
   <si>
@@ -227,9 +212,6 @@
     <t>83, 85</t>
   </si>
   <si>
-    <t>SWITCH (85-86; 100-85)</t>
-  </si>
-  <si>
     <t>84, 86</t>
   </si>
   <si>
@@ -294,6 +276,27 @@
   </si>
   <si>
     <t>STATION; CASTLE SHANNON;</t>
+  </si>
+  <si>
+    <t>STATION; OVERBROOK; UNDERGROUND; SWITCH (57-0; 57-58)</t>
+  </si>
+  <si>
+    <t>SWITCH (85-86; 85-100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATION; OVERBROOK; UNDERGROUND; </t>
+  </si>
+  <si>
+    <t>; SWITCH (63-0; 63-62)</t>
+  </si>
+  <si>
+    <t>; SWITCH (28-29; 28-150)</t>
+  </si>
+  <si>
+    <t>; SWITCH (13-1; 13-12)</t>
+  </si>
+  <si>
+    <t>STATION; MT LEBANON; SWITCH (77-76; 77-101)</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
   </sheetPr>
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -883,7 +886,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>15</v>
@@ -1153,7 +1156,7 @@
         <v>45</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>15</v>
@@ -1308,7 +1311,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="12">
@@ -1324,7 +1327,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1362,7 +1365,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1400,7 +1403,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L17" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1424,10 +1427,10 @@
         <v>70</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
@@ -1442,7 +1445,7 @@
         <v>7.7142857142857153</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1451,7 +1454,7 @@
         <v>Green</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="11">
         <v>17</v>
@@ -1480,7 +1483,7 @@
         <v>9</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1489,7 +1492,7 @@
         <v>Green</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="12">
         <v>18</v>
@@ -1518,7 +1521,7 @@
         <v>9</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1527,7 +1530,7 @@
         <v>Green</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="12">
         <v>19</v>
@@ -1542,7 +1545,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="12">
@@ -1558,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="L21" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1567,7 +1570,7 @@
         <v>Green</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="11">
         <v>20</v>
@@ -1596,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1605,7 +1608,7 @@
         <v>Green</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="12">
         <v>21</v>
@@ -1634,7 +1637,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1643,7 +1646,7 @@
         <v>Green</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="11">
         <v>22</v>
@@ -1658,10 +1661,10 @@
         <v>70</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="12">
         <f t="shared" si="0"/>
@@ -1676,7 +1679,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1685,7 +1688,7 @@
         <v>Green</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="12">
         <v>23</v>
@@ -1714,7 +1717,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1723,7 +1726,7 @@
         <v>Green</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="12">
         <v>24</v>
@@ -1752,7 +1755,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1761,7 +1764,7 @@
         <v>Green</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="11">
         <v>25</v>
@@ -1790,7 +1793,7 @@
         <v>10.285714285714286</v>
       </c>
       <c r="L27" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1799,7 +1802,7 @@
         <v>Green</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="12">
         <v>26</v>
@@ -1828,7 +1831,7 @@
         <v>5.1428571428571432</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +1840,7 @@
         <v>Green</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="11">
         <v>27</v>
@@ -1866,7 +1869,7 @@
         <v>6</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1875,7 +1878,7 @@
         <v>Green</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="12">
         <v>28</v>
@@ -1890,7 +1893,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="12">
@@ -1906,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1915,7 +1918,7 @@
         <v>Green</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" s="12">
         <v>29</v>
@@ -1953,7 +1956,7 @@
         <v>Green</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" s="11">
         <v>30</v>
@@ -1991,7 +1994,7 @@
         <v>Green</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="12">
         <v>31</v>
@@ -2006,7 +2009,7 @@
         <v>30</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>15</v>
@@ -2033,7 +2036,7 @@
         <v>Green</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="11">
         <v>32</v>
@@ -2071,7 +2074,7 @@
         <v>Green</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="12">
         <v>33</v>
@@ -2109,7 +2112,7 @@
         <v>Green</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36" s="12">
         <v>34</v>
@@ -2147,7 +2150,7 @@
         <v>Green</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="11">
         <v>35</v>
@@ -2185,7 +2188,7 @@
         <v>Green</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="12">
         <v>36</v>
@@ -2200,7 +2203,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="12">
@@ -2225,7 +2228,7 @@
         <v>Green</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" s="12">
         <v>37</v>
@@ -2240,7 +2243,7 @@
         <v>30</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="12">
@@ -2265,7 +2268,7 @@
         <v>Green</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40" s="11">
         <v>38</v>
@@ -2280,7 +2283,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="12">
@@ -2305,7 +2308,7 @@
         <v>Green</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="12">
         <v>39</v>
@@ -2320,10 +2323,10 @@
         <v>30</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I41" s="12">
         <f t="shared" si="4"/>
@@ -2347,7 +2350,7 @@
         <v>Green</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="12">
         <v>40</v>
@@ -2362,7 +2365,7 @@
         <v>30</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="12">
@@ -2387,7 +2390,7 @@
         <v>Green</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43" s="11">
         <v>41</v>
@@ -2402,7 +2405,7 @@
         <v>30</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="12">
@@ -2427,7 +2430,7 @@
         <v>Green</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C44" s="12">
         <v>42</v>
@@ -2442,7 +2445,7 @@
         <v>30</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="12">
@@ -2467,7 +2470,7 @@
         <v>Green</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45" s="12">
         <v>43</v>
@@ -2482,7 +2485,7 @@
         <v>30</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="12">
@@ -2507,7 +2510,7 @@
         <v>Green</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C46" s="11">
         <v>44</v>
@@ -2522,7 +2525,7 @@
         <v>30</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="12">
@@ -2547,7 +2550,7 @@
         <v>Green</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C47" s="12">
         <v>45</v>
@@ -2562,7 +2565,7 @@
         <v>30</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="12">
@@ -2587,7 +2590,7 @@
         <v>Green</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C48" s="12">
         <v>46</v>
@@ -2602,7 +2605,7 @@
         <v>30</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="12">
@@ -2627,7 +2630,7 @@
         <v>Green</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C49" s="11">
         <v>47</v>
@@ -2642,7 +2645,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="12">
@@ -2667,7 +2670,7 @@
         <v>Green</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C50" s="12">
         <v>48</v>
@@ -2682,10 +2685,10 @@
         <v>30</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I50" s="12">
         <f t="shared" si="4"/>
@@ -2709,7 +2712,7 @@
         <v>Green</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C51" s="12">
         <v>49</v>
@@ -2724,7 +2727,7 @@
         <v>30</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="12">
@@ -2749,7 +2752,7 @@
         <v>Green</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52" s="11">
         <v>50</v>
@@ -2764,7 +2767,7 @@
         <v>30</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="12">
@@ -2789,7 +2792,7 @@
         <v>Green</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C53" s="12">
         <v>51</v>
@@ -2804,7 +2807,7 @@
         <v>30</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="12">
@@ -2829,7 +2832,7 @@
         <v>Green</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C54" s="12">
         <v>52</v>
@@ -2844,7 +2847,7 @@
         <v>30</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="12">
@@ -2869,7 +2872,7 @@
         <v>Green</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C55" s="11">
         <v>53</v>
@@ -2884,7 +2887,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" s="12">
@@ -2909,7 +2912,7 @@
         <v>Green</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C56" s="12">
         <v>54</v>
@@ -2924,7 +2927,7 @@
         <v>30</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="12">
@@ -2949,7 +2952,7 @@
         <v>Green</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C57" s="12">
         <v>55</v>
@@ -2964,7 +2967,7 @@
         <v>30</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="12">
@@ -2989,7 +2992,7 @@
         <v>Green</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C58" s="11">
         <v>56</v>
@@ -3004,7 +3007,7 @@
         <v>30</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="12">
@@ -3029,7 +3032,7 @@
         <v>Green</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C59" s="12">
         <v>57</v>
@@ -3044,10 +3047,10 @@
         <v>30</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I59" s="12">
         <f t="shared" si="4"/>
@@ -3071,7 +3074,7 @@
         <v>Green</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C60" s="12">
         <v>58</v>
@@ -3109,7 +3112,7 @@
         <v>Green</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C61" s="11">
         <v>59</v>
@@ -3147,7 +3150,7 @@
         <v>Green</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C62" s="12">
         <v>60</v>
@@ -3185,7 +3188,7 @@
         <v>Green</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C63" s="12">
         <v>61</v>
@@ -3223,7 +3226,7 @@
         <v>Green</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C64" s="11">
         <v>62</v>
@@ -3260,7 +3263,7 @@
         <v>Green</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C65" s="12">
         <v>63</v>
@@ -3275,7 +3278,7 @@
         <v>70</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="H65" s="7"/>
       <c r="I65" s="12">
@@ -3300,7 +3303,7 @@
         <v>Green</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C66" s="12">
         <v>64</v>
@@ -3338,7 +3341,7 @@
         <v>Green</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C67" s="11">
         <v>65</v>
@@ -3353,10 +3356,10 @@
         <v>70</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I67" s="12">
         <f t="shared" ref="I67:I98" si="8">E67*D67/100</f>
@@ -3380,7 +3383,7 @@
         <v>Green</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C68" s="12">
         <v>66</v>
@@ -3418,7 +3421,7 @@
         <v>Green</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C69" s="12">
         <v>67</v>
@@ -3456,7 +3459,7 @@
         <v>Green</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C70" s="11">
         <v>68</v>
@@ -3494,7 +3497,7 @@
         <v>Green</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C71" s="12">
         <v>69</v>
@@ -3532,7 +3535,7 @@
         <v>Green</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C72" s="12">
         <v>70</v>
@@ -3570,7 +3573,7 @@
         <v>Green</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C73" s="11">
         <v>71</v>
@@ -3608,7 +3611,7 @@
         <v>Green</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C74" s="12">
         <v>72</v>
@@ -3646,7 +3649,7 @@
         <v>Green</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C75" s="12">
         <v>73</v>
@@ -3661,10 +3664,10 @@
         <v>40</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I75" s="12">
         <f t="shared" si="8"/>
@@ -3688,7 +3691,7 @@
         <v>Green</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C76" s="11">
         <v>74</v>
@@ -3726,7 +3729,7 @@
         <v>Green</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C77" s="12">
         <v>75</v>
@@ -3764,7 +3767,7 @@
         <v>Green</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C78" s="12">
         <v>76</v>
@@ -3796,13 +3799,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C79" s="12">
         <v>77</v>
@@ -3817,10 +3820,10 @@
         <v>70</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I79" s="12">
         <f t="shared" si="8"/>
@@ -3835,7 +3838,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L79" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3844,7 +3847,7 @@
         <v>Green</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C80" s="11">
         <v>78</v>
@@ -3873,7 +3876,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L80" s="18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3882,7 +3885,7 @@
         <v>Green</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C81" s="12">
         <v>79</v>
@@ -3911,7 +3914,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L81" s="18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3920,7 +3923,7 @@
         <v>Green</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C82" s="12">
         <v>80</v>
@@ -3949,7 +3952,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L82" s="18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3958,7 +3961,7 @@
         <v>Green</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C83" s="12">
         <v>81</v>
@@ -3987,7 +3990,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L83" s="18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3996,7 +3999,7 @@
         <v>Green</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C84" s="11">
         <v>82</v>
@@ -4025,7 +4028,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L84" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4034,7 +4037,7 @@
         <v>Green</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C85" s="12">
         <v>83</v>
@@ -4063,7 +4066,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L85" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4072,7 +4075,7 @@
         <v>Green</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C86" s="12">
         <v>84</v>
@@ -4101,7 +4104,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L86" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4110,7 +4113,7 @@
         <v>Green</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C87" s="12">
         <v>85</v>
@@ -4125,7 +4128,7 @@
         <v>70</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="12">
@@ -4141,7 +4144,7 @@
         <v>15.428571428571431</v>
       </c>
       <c r="L87" s="18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4150,7 +4153,7 @@
         <v>Green</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C88" s="11">
         <v>86</v>
@@ -4164,7 +4167,6 @@
       <c r="F88" s="12">
         <v>25</v>
       </c>
-      <c r="G88" s="7"/>
       <c r="H88" s="7"/>
       <c r="I88" s="12">
         <f t="shared" si="8"/>
@@ -4188,7 +4190,7 @@
         <v>Green</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C89" s="12">
         <v>87</v>
@@ -4226,7 +4228,7 @@
         <v>Green</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C90" s="12">
         <v>88</v>
@@ -4241,7 +4243,7 @@
         <v>25</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H90" s="7" t="s">
         <v>15</v>
@@ -4268,7 +4270,7 @@
         <v>Green</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C91" s="12">
         <v>89</v>
@@ -4306,7 +4308,7 @@
         <v>Green</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C92" s="11">
         <v>90</v>
@@ -4344,7 +4346,7 @@
         <v>Green</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C93" s="12">
         <v>91</v>
@@ -4382,7 +4384,7 @@
         <v>Green</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C94" s="12">
         <v>92</v>
@@ -4420,7 +4422,7 @@
         <v>Green</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C95" s="12">
         <v>93</v>
@@ -4458,7 +4460,7 @@
         <v>Green</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C96" s="11">
         <v>94</v>
@@ -4496,7 +4498,7 @@
         <v>Green</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C97" s="12">
         <v>95</v>
@@ -4528,13 +4530,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="str">
         <f t="shared" si="10"/>
         <v>Green</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C98" s="12">
         <v>96</v>
@@ -4549,7 +4551,7 @@
         <v>25</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H98" s="7" t="s">
         <v>15</v>
@@ -4576,7 +4578,7 @@
         <v>Green</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C99" s="12">
         <v>97</v>
@@ -4614,7 +4616,7 @@
         <v>Green</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C100" s="11">
         <v>98</v>
@@ -4652,7 +4654,7 @@
         <v>Green</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C101" s="12">
         <v>99</v>
@@ -4690,7 +4692,7 @@
         <v>Green</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C102" s="12">
         <v>100</v>
@@ -4728,7 +4730,7 @@
         <v>Green</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C103" s="12">
         <v>101</v>
@@ -4766,7 +4768,7 @@
         <v>Green</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C104" s="11">
         <v>102</v>
@@ -4804,7 +4806,7 @@
         <v>Green</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C105" s="12">
         <v>103</v>
@@ -4842,7 +4844,7 @@
         <v>Green</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C106" s="12">
         <v>104</v>
@@ -4880,7 +4882,7 @@
         <v>Green</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C107" s="12">
         <v>105</v>
@@ -4899,7 +4901,7 @@
         <v>STATION; DORMONT;</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I107" s="12">
         <f t="shared" si="12"/>
@@ -4923,7 +4925,7 @@
         <v>Green</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C108" s="11">
         <v>106</v>
@@ -4961,7 +4963,7 @@
         <v>Green</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C109" s="12">
         <v>107</v>
@@ -4999,7 +5001,7 @@
         <v>Green</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C110" s="12">
         <v>108</v>
@@ -5014,7 +5016,7 @@
         <v>28</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="12">
@@ -5039,7 +5041,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C111" s="12">
         <v>109</v>
@@ -5077,7 +5079,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C112" s="11">
         <v>110</v>
@@ -5115,7 +5117,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C113" s="12">
         <v>111</v>
@@ -5153,7 +5155,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C114" s="12">
         <v>112</v>
@@ -5191,7 +5193,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C115" s="12">
         <v>113</v>
@@ -5229,7 +5231,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C116" s="11">
         <v>114</v>
@@ -5248,7 +5250,7 @@
         <v>STATION; GLENBURY;</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I116" s="12">
         <f t="shared" si="12"/>
@@ -5272,7 +5274,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C117" s="12">
         <v>115</v>
@@ -5310,7 +5312,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C118" s="12">
         <v>116</v>
@@ -5348,7 +5350,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C119" s="12">
         <v>117</v>
@@ -5386,7 +5388,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C120" s="11">
         <v>118</v>
@@ -5424,7 +5426,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C121" s="12">
         <v>119</v>
@@ -5462,7 +5464,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C122" s="12">
         <v>120</v>
@@ -5500,7 +5502,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C123" s="12">
         <v>121</v>
@@ -5538,7 +5540,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C124" s="11">
         <v>122</v>
@@ -5553,7 +5555,7 @@
         <v>20</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="12">
@@ -5578,7 +5580,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C125" s="12">
         <v>123</v>
@@ -5592,12 +5594,11 @@
       <c r="F125" s="12">
         <v>20</v>
       </c>
-      <c r="G125" s="15" t="str">
-        <f>G59</f>
-        <v>STATION; OVERBROOK; UNDERGROUND; SWITCH TO YARD (57-YARD)</v>
+      <c r="G125" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I125" s="12">
         <f t="shared" si="12"/>
@@ -5621,7 +5622,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C126" s="12">
         <v>124</v>
@@ -5636,7 +5637,7 @@
         <v>20</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="12">
@@ -5661,7 +5662,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C127" s="12">
         <v>125</v>
@@ -5676,7 +5677,7 @@
         <v>20</v>
       </c>
       <c r="G127" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="12">
@@ -5701,7 +5702,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C128" s="11">
         <v>126</v>
@@ -5716,7 +5717,7 @@
         <v>20</v>
       </c>
       <c r="G128" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="12">
@@ -5741,7 +5742,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C129" s="12">
         <v>127</v>
@@ -5756,7 +5757,7 @@
         <v>20</v>
       </c>
       <c r="G129" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="12">
@@ -5781,7 +5782,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C130" s="12">
         <v>128</v>
@@ -5796,7 +5797,7 @@
         <v>20</v>
       </c>
       <c r="G130" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="12">
@@ -5821,7 +5822,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C131" s="12">
         <v>129</v>
@@ -5836,7 +5837,7 @@
         <v>20</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="12">
@@ -5861,7 +5862,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C132" s="11">
         <v>130</v>
@@ -5876,7 +5877,7 @@
         <v>20</v>
       </c>
       <c r="G132" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="12">
@@ -5901,7 +5902,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C133" s="12">
         <v>131</v>
@@ -5916,7 +5917,7 @@
         <v>20</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="12">
@@ -5941,7 +5942,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C134" s="12">
         <v>132</v>
@@ -5984,7 +5985,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C135" s="12">
         <v>133</v>
@@ -5999,7 +6000,7 @@
         <v>20</v>
       </c>
       <c r="G135" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="12">
@@ -6024,7 +6025,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C136" s="11">
         <v>134</v>
@@ -6039,7 +6040,7 @@
         <v>20</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="12">
@@ -6064,7 +6065,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C137" s="12">
         <v>135</v>
@@ -6079,7 +6080,7 @@
         <v>20</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="12">
@@ -6104,7 +6105,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C138" s="12">
         <v>136</v>
@@ -6119,7 +6120,7 @@
         <v>20</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="12">
@@ -6144,7 +6145,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C139" s="12">
         <v>137</v>
@@ -6159,7 +6160,7 @@
         <v>20</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="12">
@@ -6184,7 +6185,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C140" s="11">
         <v>138</v>
@@ -6199,7 +6200,7 @@
         <v>20</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="12">
@@ -6224,7 +6225,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C141" s="12">
         <v>139</v>
@@ -6239,7 +6240,7 @@
         <v>20</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="12">
@@ -6264,7 +6265,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C142" s="12">
         <v>140</v>
@@ -6279,7 +6280,7 @@
         <v>20</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="12">
@@ -6304,7 +6305,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C143" s="12">
         <v>141</v>
@@ -6323,7 +6324,7 @@
         <v>STATION; CENTRAL; UNDERDROUND</v>
       </c>
       <c r="H143" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I143" s="12">
         <f t="shared" si="16"/>
@@ -6347,7 +6348,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C144" s="11">
         <v>142</v>
@@ -6362,7 +6363,7 @@
         <v>20</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="12">
@@ -6387,7 +6388,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C145" s="12">
         <v>143</v>
@@ -6402,7 +6403,7 @@
         <v>20</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="12">
@@ -6427,7 +6428,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C146" s="12">
         <v>144</v>
@@ -6465,7 +6466,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C147" s="12">
         <v>145</v>
@@ -6503,7 +6504,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C148" s="11">
         <v>146</v>
@@ -6541,7 +6542,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C149" s="12">
         <v>147</v>
@@ -6579,7 +6580,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C150" s="12">
         <v>148</v>
@@ -6618,7 +6619,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C151" s="12">
         <v>149</v>
@@ -6656,7 +6657,7 @@
         <v>Green</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C152" s="11">
         <v>150</v>

</xml_diff>

<commit_message>
Arrival Times and Schedule Working
</commit_message>
<xml_diff>
--- a/CTC_Office/Green_Line_Layout.xlsx
+++ b/CTC_Office/Green_Line_Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaseckrich/Documents/Classes/ECE 1140/ECE1140_TermProject/CTC_Office/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8535BC-9056-1245-BFAB-065C6D79896C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D62575-1B5D-5F43-A92D-95C82AC6A63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -370,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,6 +435,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:N157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="B120" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K134" sqref="K134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -837,6 +840,9 @@
       <c r="L2" s="6">
         <v>63</v>
       </c>
+      <c r="M2" s="25">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -915,6 +921,9 @@
       </c>
       <c r="L4" s="6">
         <v>1</v>
+      </c>
+      <c r="M4">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1187,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="M11">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1461,7 +1470,7 @@
         <v>23</v>
       </c>
       <c r="M18">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1697,6 +1706,9 @@
       <c r="L24" s="14" t="s">
         <v>32</v>
       </c>
+      <c r="M24">
+        <v>110</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
@@ -2004,7 +2016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2045,8 +2057,11 @@
       <c r="L33" s="6">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2084,7 +2099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2122,7 +2137,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2160,7 +2175,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2198,7 +2213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="str">
         <f t="shared" si="2"/>
         <v>Green</v>
@@ -2238,7 +2253,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="str">
         <f>A35</f>
         <v>Green</v>
@@ -2278,7 +2293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="str">
         <f t="shared" ref="A40:A71" si="6">A39</f>
         <v>Green</v>
@@ -2318,7 +2333,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2359,8 +2374,11 @@
       <c r="L41" s="6">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2400,7 +2418,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2440,7 +2458,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2480,7 +2498,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2520,7 +2538,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2560,7 +2578,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2600,7 +2618,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2640,7 +2658,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2680,7 +2698,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2721,8 +2739,11 @@
       <c r="L50" s="6">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M50">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2762,7 +2783,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2802,7 +2823,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2842,7 +2863,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2882,7 +2903,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2922,7 +2943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -2962,7 +2983,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3002,7 +3023,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3042,7 +3063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3083,8 +3104,11 @@
       <c r="L59" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M59">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3122,7 +3146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3160,7 +3184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3198,7 +3222,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3236,7 +3260,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="str">
         <f t="shared" si="6"/>
         <v>Green</v>
@@ -3393,7 +3417,7 @@
         <v>66</v>
       </c>
       <c r="M67">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3704,7 +3728,7 @@
         <v>74</v>
       </c>
       <c r="M75">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3863,7 +3887,7 @@
         <v>51</v>
       </c>
       <c r="M79">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4289,7 +4313,7 @@
         <v>89</v>
       </c>
       <c r="M90">
-        <v>135</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4600,7 +4624,7 @@
         <v>97</v>
       </c>
       <c r="M98">
-        <v>52</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4950,7 +4974,7 @@
         <v>106</v>
       </c>
       <c r="M107">
-        <v>132</v>
+        <v>250</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5302,7 +5326,7 @@
         <v>115</v>
       </c>
       <c r="M116">
-        <v>64</v>
+        <v>135</v>
       </c>
     </row>
     <row r="117" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5653,7 +5677,7 @@
         <v>124</v>
       </c>
       <c r="M125">
-        <v>72</v>
+        <v>150</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6019,7 +6043,7 @@
         <v>133</v>
       </c>
       <c r="M134">
-        <v>47</v>
+        <v>105</v>
       </c>
     </row>
     <row r="135" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6385,7 +6409,7 @@
         <v>142</v>
       </c>
       <c r="M143">
-        <v>48</v>
+        <v>110</v>
       </c>
     </row>
     <row r="144" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>